<commit_message>
modified:   view/README 	modified:   view/texas/rec_poker_self.xlsx
</commit_message>
<xml_diff>
--- a/view/texas/rec_poker_self.xlsx
+++ b/view/texas/rec_poker_self.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11360" yWindow="220" windowWidth="25600" windowHeight="16000" tabRatio="755"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15940" tabRatio="755"/>
   </bookViews>
   <sheets>
     <sheet name="rec" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="410">
   <si>
     <t>user</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1534,6 +1534,38 @@
   </si>
   <si>
     <t>虾米</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全级别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>星际</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鱼儿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天府</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全聚德</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/2/4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1674,7 +1706,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1717,6 +1749,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1727,7 +1765,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="371">
+  <cellStyleXfs count="395">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2099,8 +2137,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2163,7 +2225,6 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="176" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="181" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2177,9 +2238,9 @@
     <xf numFmtId="176" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="371">
+  <cellStyles count="395">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -2365,6 +2426,18 @@
     <cellStyle name="超链接" xfId="365" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="367" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="393" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -2550,6 +2623,18 @@
     <cellStyle name="访问过的超链接" xfId="366" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="368" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="394" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
@@ -3966,13 +4051,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
+      <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -3981,15 +4066,15 @@
     <col min="2" max="2" width="9" style="43" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.1640625" style="44" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.33203125" style="45" customWidth="1"/>
-    <col min="5" max="5" width="5" style="68" customWidth="1"/>
-    <col min="6" max="7" width="5.1640625" style="68" customWidth="1"/>
-    <col min="8" max="8" width="5" style="68" customWidth="1"/>
-    <col min="9" max="9" width="2" style="68" customWidth="1"/>
-    <col min="10" max="10" width="5.5" style="69" customWidth="1"/>
-    <col min="11" max="11" width="5.5" style="70" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" style="46" customWidth="1"/>
-    <col min="13" max="13" width="5.83203125" style="67" customWidth="1"/>
-    <col min="14" max="14" width="5.1640625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="5" style="67" customWidth="1"/>
+    <col min="6" max="7" width="5.1640625" style="67" customWidth="1"/>
+    <col min="8" max="8" width="5" style="67" customWidth="1"/>
+    <col min="9" max="9" width="2" style="67" customWidth="1"/>
+    <col min="10" max="10" width="5.5" style="68" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" style="46" customWidth="1"/>
+    <col min="12" max="12" width="5.1640625" style="47" customWidth="1"/>
+    <col min="13" max="13" width="5.83203125" style="66" customWidth="1"/>
+    <col min="14" max="14" width="5.5" style="69" customWidth="1"/>
     <col min="15" max="15" width="5.83203125" style="48" customWidth="1"/>
     <col min="16" max="16" width="4.83203125" style="49" customWidth="1"/>
     <col min="17" max="17" width="12.5" style="50" bestFit="1" customWidth="1"/>
@@ -4017,35 +4102,35 @@
       <c r="D1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="70" t="s">
+      <c r="K1" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="69" t="s">
         <v>227</v>
-      </c>
-      <c r="L1" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="47" t="s">
-        <v>13</v>
       </c>
       <c r="O1" s="48" t="s">
         <v>38</v>
@@ -4116,65 +4201,65 @@
       <c r="J2" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="60">
+      <c r="K2" s="58">
+        <f>D2-174</f>
+        <v>326</v>
+      </c>
+      <c r="L2" s="55">
+        <v>42925.809027777781</v>
+      </c>
+      <c r="M2" s="66">
+        <v>326</v>
+      </c>
+      <c r="N2" s="69">
         <f>MAX($Q$2:$Q$4)/SUBTOTAL(102,$Q$2:$Q$4)</f>
         <v>1.4433333333333334</v>
-      </c>
-      <c r="L2" s="58">
-        <f>D2-174</f>
-        <v>326</v>
-      </c>
-      <c r="M2" s="58">
-        <v>326</v>
-      </c>
-      <c r="N2" s="55">
-        <v>42925.809027777781</v>
       </c>
       <c r="O2" s="48">
         <f>M2-D2</f>
         <v>-174</v>
       </c>
       <c r="P2" s="49">
-        <f>IF(L2&gt;D2,INT((L2-D2)*0.95),L2-D2)</f>
+        <f t="shared" ref="P2:P33" si="0">IF(K2&gt;D2,INT((K2-D2)*0.95),K2-D2)</f>
         <v>-174</v>
       </c>
       <c r="Q2" s="50">
-        <f>ROUND((N2-A2)*24,2)</f>
+        <f t="shared" ref="Q2:Q33" si="1">ROUND((L2-A2)*24,2)</f>
         <v>4.2699999999999996</v>
       </c>
       <c r="R2" s="50">
-        <f>G2-E2</f>
+        <f t="shared" ref="R2:R33" si="2">G2-E2</f>
         <v>249</v>
       </c>
       <c r="S2" s="50">
-        <f t="shared" ref="S2:S9" si="0">U2-T2</f>
+        <f t="shared" ref="S2:S9" si="3">U2-T2</f>
         <v>51</v>
       </c>
       <c r="T2" s="50">
-        <f>INT(E2*F2)</f>
+        <f t="shared" ref="T2:T33" si="4">INT(E2*F2)</f>
         <v>1177</v>
       </c>
       <c r="U2" s="50">
-        <f>INT(G2*H2)</f>
+        <f t="shared" ref="U2:U33" si="5">INT(G2*H2)</f>
         <v>1228</v>
       </c>
       <c r="V2" s="51">
-        <f t="shared" ref="V2:V9" si="1">S2/R2</f>
+        <f t="shared" ref="V2:V9" si="6">S2/R2</f>
         <v>0.20481927710843373</v>
       </c>
       <c r="W2" s="52">
-        <f>P2/R2*100/I2</f>
+        <f t="shared" ref="W2:W33" si="7">P2/R2*100/I2</f>
         <v>-34.939759036144579</v>
       </c>
       <c r="X2" s="52">
-        <f>P2/Q2/I2</f>
+        <f t="shared" ref="X2:X33" si="8">P2/Q2/I2</f>
         <v>-20.374707259953162</v>
       </c>
-      <c r="Y2" s="61">
-        <f>DATE(YEAR(A2),MONTH(A2),DAY(A2))</f>
+      <c r="Y2" s="60">
+        <f t="shared" ref="Y2:Y33" si="9">DATE(YEAR(A2),MONTH(A2),DAY(A2))</f>
         <v>42925</v>
       </c>
-      <c r="Z2" s="62" t="s">
+      <c r="Z2" s="61" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4209,64 +4294,64 @@
       <c r="J3" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="60">
-        <f t="shared" ref="K3:K4" si="2">MAX($Q$2:$Q$4)/SUBTOTAL(102,$Q$2:$Q$4)</f>
+      <c r="K3" s="58">
+        <v>524</v>
+      </c>
+      <c r="L3" s="55">
+        <v>42925.740972222222</v>
+      </c>
+      <c r="M3" s="66">
+        <v>508</v>
+      </c>
+      <c r="N3" s="69">
+        <f t="shared" ref="N3:N4" si="10">MAX($Q$2:$Q$4)/SUBTOTAL(102,$Q$2:$Q$4)</f>
         <v>1.4433333333333334</v>
-      </c>
-      <c r="L3" s="58">
-        <v>524</v>
-      </c>
-      <c r="M3" s="58">
-        <v>508</v>
-      </c>
-      <c r="N3" s="55">
-        <v>42925.740972222222</v>
       </c>
       <c r="O3" s="48">
         <f>M3-D3</f>
         <v>308</v>
       </c>
       <c r="P3" s="49">
-        <f>IF(L3&gt;D3,INT((L3-D3)*0.95),L3-D3)</f>
+        <f t="shared" si="0"/>
         <v>307</v>
       </c>
       <c r="Q3" s="50">
-        <f>ROUND((N3-A3)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.63</v>
       </c>
       <c r="R3" s="50">
-        <f>G3-E3</f>
+        <f t="shared" si="2"/>
         <v>166</v>
       </c>
       <c r="S3" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="T3" s="50">
-        <f>INT(E3*F3)</f>
+        <f t="shared" si="4"/>
         <v>1349</v>
       </c>
       <c r="U3" s="50">
-        <f>INT(G3*H3)</f>
+        <f t="shared" si="5"/>
         <v>1379</v>
       </c>
       <c r="V3" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.18072289156626506</v>
       </c>
       <c r="W3" s="52">
-        <f>P3/R3*100/I3</f>
+        <f t="shared" si="7"/>
         <v>92.46987951807229</v>
       </c>
       <c r="X3" s="52">
-        <f>P3/Q3/I3</f>
+        <f t="shared" si="8"/>
         <v>58.365019011406844</v>
       </c>
-      <c r="Y3" s="61">
-        <f>DATE(YEAR(A3),MONTH(A3),DAY(A3))</f>
+      <c r="Y3" s="60">
+        <f t="shared" si="9"/>
         <v>42925</v>
       </c>
-      <c r="Z3" s="62" t="s">
+      <c r="Z3" s="61" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4301,64 +4386,64 @@
       <c r="J4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="60">
-        <f t="shared" si="2"/>
+      <c r="K4" s="58">
+        <v>367</v>
+      </c>
+      <c r="L4" s="55">
+        <v>42925.811805555553</v>
+      </c>
+      <c r="M4" s="66">
+        <v>367</v>
+      </c>
+      <c r="N4" s="69">
+        <f t="shared" si="10"/>
         <v>1.4433333333333334</v>
-      </c>
-      <c r="L4" s="58">
-        <v>367</v>
-      </c>
-      <c r="M4" s="58">
-        <v>367</v>
-      </c>
-      <c r="N4" s="55">
-        <v>42925.811805555553</v>
       </c>
       <c r="O4" s="48">
         <f>M4-D4</f>
         <v>67</v>
       </c>
       <c r="P4" s="49">
-        <f>IF(L4&gt;D4,INT((L4-D4)*0.95),L4-D4)</f>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="Q4" s="50">
-        <f>ROUND((N4-A4)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>4.33</v>
       </c>
       <c r="R4" s="50">
-        <f>G4-E4</f>
+        <f t="shared" si="2"/>
         <v>244</v>
       </c>
       <c r="S4" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="T4" s="50">
-        <f>INT(E4*F4)</f>
+        <f t="shared" si="4"/>
         <v>1071</v>
       </c>
       <c r="U4" s="50">
-        <f>INT(G4*H4)</f>
+        <f t="shared" si="5"/>
         <v>1121</v>
       </c>
       <c r="V4" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.20491803278688525</v>
       </c>
       <c r="W4" s="52">
-        <f>P4/R4*100/I4</f>
+        <f t="shared" si="7"/>
         <v>12.909836065573771</v>
       </c>
       <c r="X4" s="52">
-        <f>P4/Q4/I4</f>
+        <f t="shared" si="8"/>
         <v>7.274826789838337</v>
       </c>
-      <c r="Y4" s="61">
-        <f>DATE(YEAR(A4),MONTH(A4),DAY(A4))</f>
+      <c r="Y4" s="60">
+        <f t="shared" si="9"/>
         <v>42925</v>
       </c>
-      <c r="Z4" s="62" t="s">
+      <c r="Z4" s="61" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4376,80 +4461,80 @@
         <f>200+100</f>
         <v>300</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="67">
         <v>2186</v>
       </c>
-      <c r="F5" s="68">
+      <c r="F5" s="67">
         <v>0.66</v>
       </c>
-      <c r="G5" s="68">
+      <c r="G5" s="67">
         <v>2320</v>
       </c>
-      <c r="H5" s="68">
+      <c r="H5" s="67">
         <v>0.63</v>
       </c>
-      <c r="I5" s="68">
+      <c r="I5" s="67">
         <v>2</v>
       </c>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="70">
+      <c r="K5" s="46">
+        <f>D5+108</f>
+        <v>408</v>
+      </c>
+      <c r="L5" s="47">
+        <v>42935.022222222222</v>
+      </c>
+      <c r="M5" s="66">
+        <v>403</v>
+      </c>
+      <c r="N5" s="69">
         <f>MAX($Q$5:$Q$9)/SUBTOTAL(102,$Q$5:$Q$9)</f>
         <v>0.79400000000000004</v>
-      </c>
-      <c r="L5" s="46">
-        <f>D5+108</f>
-        <v>408</v>
-      </c>
-      <c r="M5" s="67">
-        <v>403</v>
-      </c>
-      <c r="N5" s="47">
-        <v>42935.022222222222</v>
       </c>
       <c r="O5" s="48">
         <f>MAX($Q$5:$Q$9)/5</f>
         <v>0.79400000000000004</v>
       </c>
       <c r="P5" s="49">
-        <f>IF(L5&gt;D5,INT((L5-D5)*0.95),L5-D5)</f>
+        <f t="shared" si="0"/>
         <v>102</v>
       </c>
       <c r="Q5" s="50">
-        <f>ROUND((N5-A5)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
       <c r="R5" s="50">
-        <f>G5-E5</f>
+        <f t="shared" si="2"/>
         <v>134</v>
       </c>
       <c r="S5" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="T5" s="50">
-        <f>INT(E5*F5)</f>
+        <f t="shared" si="4"/>
         <v>1442</v>
       </c>
       <c r="U5" s="50">
-        <f>INT(G5*H5)</f>
+        <f t="shared" si="5"/>
         <v>1461</v>
       </c>
       <c r="V5" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.1417910447761194</v>
       </c>
       <c r="W5" s="52">
-        <f>P5/R5*100/I5</f>
+        <f t="shared" si="7"/>
         <v>38.059701492537314</v>
       </c>
       <c r="X5" s="52">
-        <f>P5/Q5/I5</f>
+        <f t="shared" si="8"/>
         <v>14.571428571428571</v>
       </c>
       <c r="Y5" s="53">
-        <f>DATE(YEAR(A5),MONTH(A5),DAY(A5))</f>
+        <f t="shared" si="9"/>
         <v>42934</v>
       </c>
       <c r="Z5" s="54" t="s">
@@ -4469,80 +4554,80 @@
       <c r="D6" s="44">
         <v>200</v>
       </c>
-      <c r="E6" s="68">
+      <c r="E6" s="67">
         <v>2584</v>
       </c>
-      <c r="F6" s="68">
+      <c r="F6" s="67">
         <v>0.62</v>
       </c>
-      <c r="G6" s="68">
+      <c r="G6" s="67">
         <v>2816</v>
       </c>
-      <c r="H6" s="68">
+      <c r="H6" s="67">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I6" s="68">
+      <c r="I6" s="67">
         <v>2</v>
       </c>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="70">
-        <f t="shared" ref="K6:K9" si="3">MAX($Q$5:$Q$9)/SUBTOTAL(102,$Q$5:$Q$9)</f>
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="L6" s="46">
+      <c r="K6" s="46">
         <f>D6+7</f>
         <v>207</v>
       </c>
-      <c r="M6" s="67">
+      <c r="L6" s="47">
+        <v>42935.041666666664</v>
+      </c>
+      <c r="M6" s="66">
         <v>207</v>
       </c>
-      <c r="N6" s="47">
-        <v>42935.041666666664</v>
+      <c r="N6" s="69">
+        <f t="shared" ref="N6:N9" si="11">MAX($Q$5:$Q$9)/SUBTOTAL(102,$Q$5:$Q$9)</f>
+        <v>0.79400000000000004</v>
       </c>
       <c r="O6" s="48">
         <f>MAX($Q$5:$Q$9)/5</f>
         <v>0.79400000000000004</v>
       </c>
       <c r="P6" s="49">
-        <f>IF(L6&gt;D6,INT((L6-D6)*0.95),L6-D6)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="Q6" s="50">
-        <f>ROUND((N6-A6)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>3.97</v>
       </c>
       <c r="R6" s="50">
-        <f>G6-E6</f>
+        <f t="shared" si="2"/>
         <v>232</v>
       </c>
       <c r="S6" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="T6" s="50">
-        <f>INT(E6*F6)</f>
+        <f t="shared" si="4"/>
         <v>1602</v>
       </c>
       <c r="U6" s="50">
-        <f>INT(G6*H6)</f>
+        <f t="shared" si="5"/>
         <v>1633</v>
       </c>
       <c r="V6" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.1336206896551724</v>
       </c>
       <c r="W6" s="52">
-        <f>P6/R6*100/I6</f>
+        <f t="shared" si="7"/>
         <v>1.2931034482758621</v>
       </c>
       <c r="X6" s="52">
-        <f>P6/Q6/I6</f>
+        <f t="shared" si="8"/>
         <v>0.75566750629722923</v>
       </c>
       <c r="Y6" s="53">
-        <f>DATE(YEAR(A6),MONTH(A6),DAY(A6))</f>
+        <f t="shared" si="9"/>
         <v>42934</v>
       </c>
       <c r="Z6" s="54" t="s">
@@ -4563,80 +4648,80 @@
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="E7" s="68">
+      <c r="E7" s="67">
         <v>1753</v>
       </c>
-      <c r="F7" s="68">
+      <c r="F7" s="67">
         <v>0.64</v>
       </c>
-      <c r="G7" s="68">
+      <c r="G7" s="67">
         <v>1855</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="67">
         <v>0.61</v>
       </c>
-      <c r="I7" s="68">
+      <c r="I7" s="67">
         <v>4</v>
       </c>
-      <c r="J7" s="69" t="s">
+      <c r="J7" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="K7" s="70">
-        <f t="shared" si="3"/>
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="L7" s="46">
+      <c r="K7" s="46">
         <f>D7+618</f>
         <v>1018</v>
       </c>
-      <c r="M7" s="67">
+      <c r="L7" s="47">
+        <v>42934.955555555556</v>
+      </c>
+      <c r="M7" s="66">
         <v>988</v>
       </c>
-      <c r="N7" s="47">
-        <v>42934.955555555556</v>
+      <c r="N7" s="69">
+        <f t="shared" si="11"/>
+        <v>0.79400000000000004</v>
       </c>
       <c r="O7" s="48">
-        <f>M7-D7</f>
+        <f t="shared" ref="O7:O33" si="12">M7-D7</f>
         <v>588</v>
       </c>
       <c r="P7" s="49">
-        <f>IF(L7&gt;D7,INT((L7-D7)*0.95),L7-D7)</f>
+        <f t="shared" si="0"/>
         <v>587</v>
       </c>
       <c r="Q7" s="50">
-        <f>ROUND((N7-A7)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>1.9</v>
       </c>
       <c r="R7" s="50">
-        <f>G7-E7</f>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="S7" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="T7" s="50">
-        <f>INT(E7*F7)</f>
+        <f t="shared" si="4"/>
         <v>1121</v>
       </c>
       <c r="U7" s="50">
-        <f>INT(G7*H7)</f>
+        <f t="shared" si="5"/>
         <v>1131</v>
       </c>
       <c r="V7" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>9.8039215686274508E-2</v>
       </c>
       <c r="W7" s="52">
-        <f>P7/R7*100/I7</f>
+        <f t="shared" si="7"/>
         <v>143.87254901960785</v>
       </c>
       <c r="X7" s="52">
-        <f>P7/Q7/I7</f>
+        <f t="shared" si="8"/>
         <v>77.236842105263165</v>
       </c>
       <c r="Y7" s="53">
-        <f>DATE(YEAR(A7),MONTH(A7),DAY(A7))</f>
+        <f t="shared" si="9"/>
         <v>42934</v>
       </c>
       <c r="Z7" s="54" t="s">
@@ -4656,80 +4741,80 @@
       <c r="D8" s="44">
         <v>200</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="67">
         <v>1674</v>
       </c>
-      <c r="F8" s="68">
+      <c r="F8" s="67">
         <v>0.63</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="67">
         <v>1830</v>
       </c>
-      <c r="H8" s="68">
+      <c r="H8" s="67">
         <v>0.6</v>
       </c>
-      <c r="I8" s="68">
+      <c r="I8" s="67">
         <v>2</v>
       </c>
-      <c r="J8" s="69" t="s">
+      <c r="J8" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="70">
-        <f t="shared" si="3"/>
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="L8" s="46">
+      <c r="K8" s="46">
         <f>D8+32</f>
         <v>232</v>
       </c>
-      <c r="M8" s="67">
+      <c r="L8" s="47">
+        <v>42934.986805555556</v>
+      </c>
+      <c r="M8" s="66">
         <v>232</v>
       </c>
-      <c r="N8" s="47">
-        <v>42934.986805555556</v>
+      <c r="N8" s="69">
+        <f t="shared" si="11"/>
+        <v>0.79400000000000004</v>
       </c>
       <c r="O8" s="48">
-        <f>M8-D8</f>
+        <f t="shared" si="12"/>
         <v>32</v>
       </c>
       <c r="P8" s="49">
-        <f>IF(L8&gt;D8,INT((L8-D8)*0.95),L8-D8)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="Q8" s="50">
-        <f>ROUND((N8-A8)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.65</v>
       </c>
       <c r="R8" s="50">
-        <f>G8-E8</f>
+        <f t="shared" si="2"/>
         <v>156</v>
       </c>
       <c r="S8" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>44</v>
       </c>
       <c r="T8" s="50">
-        <f>INT(E8*F8)</f>
+        <f t="shared" si="4"/>
         <v>1054</v>
       </c>
       <c r="U8" s="50">
-        <f>INT(G8*H8)</f>
+        <f t="shared" si="5"/>
         <v>1098</v>
       </c>
       <c r="V8" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.28205128205128205</v>
       </c>
       <c r="W8" s="52">
-        <f>P8/R8*100/I8</f>
+        <f t="shared" si="7"/>
         <v>9.6153846153846168</v>
       </c>
       <c r="X8" s="52">
-        <f>P8/Q8/I8</f>
+        <f t="shared" si="8"/>
         <v>5.6603773584905666</v>
       </c>
       <c r="Y8" s="53">
-        <f>DATE(YEAR(A8),MONTH(A8),DAY(A8))</f>
+        <f t="shared" si="9"/>
         <v>42934</v>
       </c>
       <c r="Z8" s="54" t="s">
@@ -4749,80 +4834,80 @@
       <c r="D9" s="44">
         <v>200</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="67">
         <v>1855</v>
       </c>
-      <c r="F9" s="68">
+      <c r="F9" s="67">
         <v>0.61</v>
       </c>
-      <c r="G9" s="68">
+      <c r="G9" s="67">
         <v>1967</v>
       </c>
-      <c r="H9" s="68">
+      <c r="H9" s="67">
         <v>0.59</v>
       </c>
-      <c r="I9" s="68">
+      <c r="I9" s="67">
         <v>2</v>
       </c>
-      <c r="J9" s="69" t="s">
+      <c r="J9" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="70">
-        <f t="shared" si="3"/>
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="L9" s="46">
+      <c r="K9" s="46">
         <f>D9+177</f>
         <v>377</v>
       </c>
-      <c r="M9" s="67">
+      <c r="L9" s="47">
+        <v>42935.03402777778</v>
+      </c>
+      <c r="M9" s="66">
         <v>369</v>
       </c>
-      <c r="N9" s="47">
-        <v>42935.03402777778</v>
+      <c r="N9" s="69">
+        <f t="shared" si="11"/>
+        <v>0.79400000000000004</v>
       </c>
       <c r="O9" s="48">
-        <f>M9-D9</f>
+        <f t="shared" si="12"/>
         <v>169</v>
       </c>
       <c r="P9" s="49">
-        <f>IF(L9&gt;D9,INT((L9-D9)*0.95),L9-D9)</f>
+        <f t="shared" si="0"/>
         <v>168</v>
       </c>
       <c r="Q9" s="50">
-        <f>ROUND((N9-A9)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>1.88</v>
       </c>
       <c r="R9" s="50">
-        <f>G9-E9</f>
+        <f t="shared" si="2"/>
         <v>112</v>
       </c>
       <c r="S9" s="50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="T9" s="50">
-        <f>INT(E9*F9)</f>
+        <f t="shared" si="4"/>
         <v>1131</v>
       </c>
       <c r="U9" s="50">
-        <f>INT(G9*H9)</f>
+        <f t="shared" si="5"/>
         <v>1160</v>
       </c>
       <c r="V9" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>0.25892857142857145</v>
       </c>
       <c r="W9" s="52">
-        <f>P9/R9*100/I9</f>
+        <f t="shared" si="7"/>
         <v>75</v>
       </c>
       <c r="X9" s="52">
-        <f>P9/Q9/I9</f>
+        <f t="shared" si="8"/>
         <v>44.680851063829792</v>
       </c>
       <c r="Y9" s="53">
-        <f>DATE(YEAR(A9),MONTH(A9),DAY(A9))</f>
+        <f t="shared" si="9"/>
         <v>42934</v>
       </c>
       <c r="Z9" s="54" t="s">
@@ -4861,65 +4946,65 @@
       <c r="J10" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="60">
+      <c r="K10" s="58">
+        <f>D10+150</f>
+        <v>350</v>
+      </c>
+      <c r="L10" s="55">
+        <v>42936.959722222222</v>
+      </c>
+      <c r="M10" s="66">
+        <v>342</v>
+      </c>
+      <c r="N10" s="69">
         <f>MAX($Q$10:$Q$11)/SUBTOTAL(102,$Q$10:$Q$11)</f>
         <v>1.3149999999999999</v>
       </c>
-      <c r="L10" s="58">
-        <f>D10+150</f>
-        <v>350</v>
-      </c>
-      <c r="M10" s="58">
-        <v>342</v>
-      </c>
-      <c r="N10" s="55">
-        <v>42936.959722222222</v>
-      </c>
       <c r="O10" s="48">
-        <f>M10-D10</f>
+        <f t="shared" si="12"/>
         <v>142</v>
       </c>
       <c r="P10" s="49">
-        <f>IF(L10&gt;D10,INT((L10-D10)*0.95),L10-D10)</f>
+        <f t="shared" si="0"/>
         <v>142</v>
       </c>
       <c r="Q10" s="50">
-        <f>ROUND((N10-A10)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="R10" s="50">
-        <f>G10-E10</f>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="S10" s="50">
-        <f t="shared" ref="S10:S14" si="4">U10-T10</f>
+        <f t="shared" ref="S10:S14" si="13">U10-T10</f>
         <v>16</v>
       </c>
       <c r="T10" s="50">
-        <f>INT(E10*F10)</f>
+        <f t="shared" si="4"/>
         <v>1461</v>
       </c>
       <c r="U10" s="50">
-        <f>INT(G10*H10)</f>
+        <f t="shared" si="5"/>
         <v>1477</v>
       </c>
       <c r="V10" s="51">
-        <f t="shared" ref="V10" si="5">S10/R10</f>
+        <f t="shared" ref="V10" si="14">S10/R10</f>
         <v>0.15686274509803921</v>
       </c>
       <c r="W10" s="52">
-        <f>P10/R10*100/I10</f>
+        <f t="shared" si="7"/>
         <v>69.607843137254903</v>
       </c>
       <c r="X10" s="52">
-        <f>P10/Q10/I10</f>
+        <f t="shared" si="8"/>
         <v>28.4</v>
       </c>
-      <c r="Y10" s="61">
-        <f>DATE(YEAR(A10),MONTH(A10),DAY(A10))</f>
+      <c r="Y10" s="60">
+        <f t="shared" si="9"/>
         <v>42936</v>
       </c>
-      <c r="Z10" s="62" t="s">
+      <c r="Z10" s="61" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4955,46 +5040,46 @@
       <c r="J11" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="60">
+      <c r="K11" s="58">
+        <f>D11-132</f>
+        <v>268</v>
+      </c>
+      <c r="L11" s="55">
+        <v>42936.965277777781</v>
+      </c>
+      <c r="M11" s="66">
+        <v>268</v>
+      </c>
+      <c r="N11" s="69">
         <f>MAX($Q$10:$Q$11)/SUBTOTAL(102,$Q$10:$Q$11)</f>
         <v>1.3149999999999999</v>
       </c>
-      <c r="L11" s="58">
-        <f>D11-132</f>
-        <v>268</v>
-      </c>
-      <c r="M11" s="58">
-        <v>268</v>
-      </c>
-      <c r="N11" s="55">
-        <v>42936.965277777781</v>
-      </c>
       <c r="O11" s="48">
-        <f>M11-D11</f>
+        <f t="shared" si="12"/>
         <v>-132</v>
       </c>
       <c r="P11" s="49">
-        <f>IF(L11&gt;D11,INT((L11-D11)*0.95),L11-D11)</f>
+        <f t="shared" si="0"/>
         <v>-132</v>
       </c>
       <c r="Q11" s="50">
-        <f>ROUND((N11-A11)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.63</v>
       </c>
       <c r="R11" s="50">
-        <f>G11-E11</f>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="S11" s="50">
+        <f t="shared" si="13"/>
+        <v>46</v>
+      </c>
+      <c r="T11" s="50">
         <f t="shared" si="4"/>
-        <v>46</v>
-      </c>
-      <c r="T11" s="50">
-        <f>INT(E11*F11)</f>
         <v>1160</v>
       </c>
       <c r="U11" s="50">
-        <f>INT(G11*H11)</f>
+        <f t="shared" si="5"/>
         <v>1206</v>
       </c>
       <c r="V11" s="51">
@@ -5002,18 +5087,18 @@
         <v>0.30666666666666664</v>
       </c>
       <c r="W11" s="52">
-        <f>P11/R11*100/I11</f>
+        <f t="shared" si="7"/>
         <v>-44</v>
       </c>
       <c r="X11" s="52">
-        <f>P11/Q11/I11</f>
+        <f t="shared" si="8"/>
         <v>-25.095057034220535</v>
       </c>
-      <c r="Y11" s="61">
-        <f>DATE(YEAR(A11),MONTH(A11),DAY(A11))</f>
+      <c r="Y11" s="60">
+        <f t="shared" si="9"/>
         <v>42936</v>
       </c>
-      <c r="Z11" s="62" t="s">
+      <c r="Z11" s="61" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5031,79 +5116,79 @@
         <f>200</f>
         <v>200</v>
       </c>
-      <c r="E12" s="68">
+      <c r="E12" s="67">
         <v>2816</v>
       </c>
-      <c r="F12" s="68">
+      <c r="F12" s="67">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G12" s="68">
+      <c r="G12" s="67">
         <v>2997</v>
       </c>
-      <c r="H12" s="68">
+      <c r="H12" s="67">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I12" s="68">
+      <c r="I12" s="67">
         <v>2</v>
       </c>
-      <c r="J12" s="69" t="s">
+      <c r="J12" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="70">
+      <c r="K12" s="46">
+        <v>189</v>
+      </c>
+      <c r="L12" s="47">
+        <v>42939.000011574077</v>
+      </c>
+      <c r="M12" s="66">
+        <v>189</v>
+      </c>
+      <c r="N12" s="69">
         <f>MAX($Q$12:$Q$15)/SUBTOTAL(102,$Q$12:$Q$15)</f>
         <v>0.74250000000000005</v>
       </c>
-      <c r="L12" s="46">
-        <v>189</v>
-      </c>
-      <c r="M12" s="67">
-        <v>189</v>
-      </c>
-      <c r="N12" s="47">
-        <v>42939.000011574077</v>
-      </c>
       <c r="O12" s="48">
-        <f>M12-D12</f>
+        <f t="shared" si="12"/>
         <v>-11</v>
       </c>
       <c r="P12" s="49">
-        <f>IF(L12&gt;D12,INT((L12-D12)*0.95),L12-D12)</f>
+        <f t="shared" si="0"/>
         <v>-11</v>
       </c>
       <c r="Q12" s="50">
-        <f>ROUND((N12-A12)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.92</v>
       </c>
       <c r="R12" s="50">
-        <f>G12-E12</f>
+        <f t="shared" si="2"/>
         <v>181</v>
       </c>
       <c r="S12" s="50">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="T12" s="50">
         <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="T12" s="50">
-        <f>INT(E12*F12)</f>
         <v>1633</v>
       </c>
       <c r="U12" s="50">
-        <f>INT(G12*H12)</f>
+        <f t="shared" si="5"/>
         <v>1648</v>
       </c>
       <c r="V12" s="51">
-        <f t="shared" ref="V12:V15" si="6">S12/R12</f>
+        <f t="shared" ref="V12:V15" si="15">S12/R12</f>
         <v>8.2872928176795577E-2</v>
       </c>
       <c r="W12" s="52">
-        <f>P12/R12*100/I12</f>
+        <f t="shared" si="7"/>
         <v>-3.0386740331491713</v>
       </c>
       <c r="X12" s="52">
-        <f>P12/Q12/I12</f>
+        <f t="shared" si="8"/>
         <v>-1.8835616438356164</v>
       </c>
       <c r="Y12" s="53">
-        <f>DATE(YEAR(A12),MONTH(A12),DAY(A12))</f>
+        <f t="shared" si="9"/>
         <v>42938</v>
       </c>
       <c r="Z12" s="54" t="s">
@@ -5124,80 +5209,80 @@
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="E13" s="68">
+      <c r="E13" s="67">
         <v>1830</v>
       </c>
-      <c r="F13" s="68">
+      <c r="F13" s="67">
         <v>0.6</v>
       </c>
-      <c r="G13" s="68">
+      <c r="G13" s="67">
         <v>1994</v>
       </c>
-      <c r="H13" s="68">
+      <c r="H13" s="67">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I13" s="68">
+      <c r="I13" s="67">
         <v>4</v>
       </c>
-      <c r="J13" s="69" t="s">
+      <c r="J13" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="K13" s="70">
-        <f t="shared" ref="K13:K15" si="7">MAX($Q$12:$Q$15)/SUBTOTAL(102,$Q$12:$Q$15)</f>
-        <v>0.74250000000000005</v>
-      </c>
-      <c r="L13" s="46">
+      <c r="K13" s="46">
         <f>D13+274</f>
         <v>674</v>
       </c>
-      <c r="M13" s="67">
+      <c r="L13" s="47">
+        <v>42938.982638888891</v>
+      </c>
+      <c r="M13" s="66">
         <v>665</v>
       </c>
-      <c r="N13" s="47">
-        <v>42938.982638888891</v>
+      <c r="N13" s="69">
+        <f t="shared" ref="N13:N15" si="16">MAX($Q$12:$Q$15)/SUBTOTAL(102,$Q$12:$Q$15)</f>
+        <v>0.74250000000000005</v>
       </c>
       <c r="O13" s="48">
-        <f>M13-D13</f>
+        <f t="shared" si="12"/>
         <v>265</v>
       </c>
       <c r="P13" s="49">
-        <f>IF(L13&gt;D13,INT((L13-D13)*0.95),L13-D13)</f>
+        <f t="shared" si="0"/>
         <v>260</v>
       </c>
       <c r="Q13" s="50">
-        <f>ROUND((N13-A13)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="R13" s="50">
-        <f>G13-E13</f>
+        <f t="shared" si="2"/>
         <v>164</v>
       </c>
       <c r="S13" s="50">
+        <f t="shared" si="13"/>
+        <v>18</v>
+      </c>
+      <c r="T13" s="50">
         <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="T13" s="50">
-        <f>INT(E13*F13)</f>
         <v>1098</v>
       </c>
       <c r="U13" s="50">
-        <f>INT(G13*H13)</f>
+        <f t="shared" si="5"/>
         <v>1116</v>
       </c>
       <c r="V13" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.10975609756097561</v>
       </c>
       <c r="W13" s="52">
-        <f>P13/R13*100/I13</f>
+        <f t="shared" si="7"/>
         <v>39.634146341463413</v>
       </c>
       <c r="X13" s="52">
-        <f>P13/Q13/I13</f>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="Y13" s="53">
-        <f>DATE(YEAR(A13),MONTH(A13),DAY(A13))</f>
+        <f t="shared" si="9"/>
         <v>42938</v>
       </c>
       <c r="Z13" s="54" t="s">
@@ -5218,80 +5303,80 @@
         <f>400+400+1000</f>
         <v>1800</v>
       </c>
-      <c r="E14" s="68">
+      <c r="E14" s="67">
         <v>2117</v>
       </c>
-      <c r="F14" s="68">
+      <c r="F14" s="67">
         <v>0.56999999999999995</v>
       </c>
-      <c r="G14" s="68">
+      <c r="G14" s="67">
         <v>2265</v>
       </c>
-      <c r="H14" s="68">
+      <c r="H14" s="67">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I14" s="68">
+      <c r="I14" s="67">
         <v>4</v>
       </c>
-      <c r="J14" s="69" t="s">
+      <c r="J14" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="K14" s="70">
-        <f t="shared" si="7"/>
-        <v>0.74250000000000005</v>
-      </c>
-      <c r="L14" s="46">
+      <c r="K14" s="46">
         <f>D14-828</f>
         <v>972</v>
       </c>
-      <c r="M14" s="67">
+      <c r="L14" s="47">
+        <v>42938.988888888889</v>
+      </c>
+      <c r="M14" s="66">
         <v>972</v>
       </c>
-      <c r="N14" s="47">
-        <v>42938.988888888889</v>
+      <c r="N14" s="69">
+        <f t="shared" si="16"/>
+        <v>0.74250000000000005</v>
       </c>
       <c r="O14" s="48">
-        <f>M14-D14</f>
+        <f t="shared" si="12"/>
         <v>-828</v>
       </c>
       <c r="P14" s="49">
-        <f>IF(L14&gt;D14,INT((L14-D14)*0.95),L14-D14)</f>
+        <f t="shared" si="0"/>
         <v>-828</v>
       </c>
       <c r="Q14" s="50">
-        <f>ROUND((N14-A14)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.52</v>
       </c>
       <c r="R14" s="50">
-        <f>G14-E14</f>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="S14" s="50">
+        <f t="shared" si="13"/>
+        <v>39</v>
+      </c>
+      <c r="T14" s="50">
         <f t="shared" si="4"/>
-        <v>39</v>
-      </c>
-      <c r="T14" s="50">
-        <f>INT(E14*F14)</f>
         <v>1206</v>
       </c>
       <c r="U14" s="50">
-        <f>INT(G14*H14)</f>
+        <f t="shared" si="5"/>
         <v>1245</v>
       </c>
       <c r="V14" s="51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.26351351351351349</v>
       </c>
       <c r="W14" s="52">
-        <f>P14/R14*100/I14</f>
+        <f t="shared" si="7"/>
         <v>-139.86486486486487</v>
       </c>
       <c r="X14" s="52">
-        <f>P14/Q14/I14</f>
+        <f t="shared" si="8"/>
         <v>-82.142857142857139</v>
       </c>
       <c r="Y14" s="53">
-        <f>DATE(YEAR(A14),MONTH(A14),DAY(A14))</f>
+        <f t="shared" si="9"/>
         <v>42938</v>
       </c>
       <c r="Z14" s="54" t="s">
@@ -5311,79 +5396,79 @@
       <c r="D15" s="44">
         <v>200</v>
       </c>
-      <c r="E15" s="68">
+      <c r="E15" s="67">
         <v>2422</v>
       </c>
-      <c r="F15" s="68">
+      <c r="F15" s="67">
         <v>0.61</v>
       </c>
-      <c r="G15" s="68">
+      <c r="G15" s="67">
         <v>2557</v>
       </c>
-      <c r="H15" s="68">
+      <c r="H15" s="67">
         <v>0.59</v>
       </c>
-      <c r="I15" s="68">
+      <c r="I15" s="67">
         <v>2</v>
       </c>
-      <c r="J15" s="69" t="s">
+      <c r="J15" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="70">
+      <c r="K15" s="46">
+        <v>215</v>
+      </c>
+      <c r="L15" s="47">
+        <v>42939.000011574077</v>
+      </c>
+      <c r="M15" s="66">
+        <v>215</v>
+      </c>
+      <c r="N15" s="69">
+        <f t="shared" si="16"/>
+        <v>0.74250000000000005</v>
+      </c>
+      <c r="O15" s="48">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="P15" s="49">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Q15" s="50">
+        <f t="shared" si="1"/>
+        <v>2.97</v>
+      </c>
+      <c r="R15" s="50">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="S15" s="50">
+        <f t="shared" ref="S15" si="17">U15-T15</f>
+        <v>31</v>
+      </c>
+      <c r="T15" s="50">
+        <f t="shared" si="4"/>
+        <v>1477</v>
+      </c>
+      <c r="U15" s="50">
+        <f t="shared" si="5"/>
+        <v>1508</v>
+      </c>
+      <c r="V15" s="51">
+        <f t="shared" si="15"/>
+        <v>0.22962962962962963</v>
+      </c>
+      <c r="W15" s="52">
         <f t="shared" si="7"/>
-        <v>0.74250000000000005</v>
-      </c>
-      <c r="L15" s="46">
-        <v>215</v>
-      </c>
-      <c r="M15" s="67">
-        <v>215</v>
-      </c>
-      <c r="N15" s="47">
-        <v>42939.000011574077</v>
-      </c>
-      <c r="O15" s="48">
-        <f>M15-D15</f>
-        <v>15</v>
-      </c>
-      <c r="P15" s="49">
-        <f>IF(L15&gt;D15,INT((L15-D15)*0.95),L15-D15)</f>
-        <v>14</v>
-      </c>
-      <c r="Q15" s="50">
-        <f>ROUND((N15-A15)*24,2)</f>
-        <v>2.97</v>
-      </c>
-      <c r="R15" s="50">
-        <f>G15-E15</f>
-        <v>135</v>
-      </c>
-      <c r="S15" s="50">
-        <f t="shared" ref="S15" si="8">U15-T15</f>
-        <v>31</v>
-      </c>
-      <c r="T15" s="50">
-        <f>INT(E15*F15)</f>
-        <v>1477</v>
-      </c>
-      <c r="U15" s="50">
-        <f>INT(G15*H15)</f>
-        <v>1508</v>
-      </c>
-      <c r="V15" s="51">
-        <f t="shared" si="6"/>
-        <v>0.22962962962962963</v>
-      </c>
-      <c r="W15" s="52">
-        <f>P15/R15*100/I15</f>
         <v>5.1851851851851851</v>
       </c>
       <c r="X15" s="52">
-        <f>P15/Q15/I15</f>
+        <f t="shared" si="8"/>
         <v>2.3569023569023568</v>
       </c>
       <c r="Y15" s="53">
-        <f>DATE(YEAR(A15),MONTH(A15),DAY(A15))</f>
+        <f t="shared" si="9"/>
         <v>42938</v>
       </c>
       <c r="Z15" s="54" t="s">
@@ -5422,34 +5507,34 @@
       <c r="J16" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="K16" s="60">
+      <c r="K16" s="58">
+        <f>D16-318</f>
+        <v>582</v>
+      </c>
+      <c r="L16" s="55">
+        <v>42946.729861111111</v>
+      </c>
+      <c r="M16" s="66">
+        <v>582</v>
+      </c>
+      <c r="N16" s="69">
         <f>MAX($Q$16:$Q$18)/SUBTOTAL(102,$Q$16:$Q$18)</f>
         <v>0.84</v>
       </c>
-      <c r="L16" s="58">
-        <f>D16-318</f>
-        <v>582</v>
-      </c>
-      <c r="M16" s="58">
-        <v>582</v>
-      </c>
-      <c r="N16" s="55">
-        <v>42946.729861111111</v>
-      </c>
       <c r="O16" s="48">
-        <f>M16-D16</f>
+        <f t="shared" si="12"/>
         <v>-318</v>
       </c>
       <c r="P16" s="49">
-        <f>IF(L16&gt;D16,INT((L16-D16)*0.95),L16-D16)</f>
+        <f t="shared" si="0"/>
         <v>-318</v>
       </c>
       <c r="Q16" s="50">
-        <f>ROUND((N16-A16)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.52</v>
       </c>
       <c r="R16" s="50">
-        <f>G16-E16</f>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="S16" s="50">
@@ -5457,30 +5542,30 @@
         <v>26</v>
       </c>
       <c r="T16" s="50">
-        <f>INT(E16*F16)</f>
+        <f t="shared" si="4"/>
         <v>2008</v>
       </c>
       <c r="U16" s="50">
-        <f>INT(G16*H16)</f>
+        <f t="shared" si="5"/>
         <v>2034</v>
       </c>
       <c r="V16" s="51">
-        <f t="shared" ref="V16:V18" si="9">S16/R16</f>
+        <f t="shared" ref="V16:V18" si="18">S16/R16</f>
         <v>0.16250000000000001</v>
       </c>
       <c r="W16" s="52">
-        <f>P16/R16*100/I16</f>
+        <f t="shared" si="7"/>
         <v>-49.6875</v>
       </c>
       <c r="X16" s="52">
-        <f>P16/Q16/I16</f>
+        <f t="shared" si="8"/>
         <v>-31.547619047619047</v>
       </c>
-      <c r="Y16" s="61">
-        <f>DATE(YEAR(A16),MONTH(A16),DAY(A16))</f>
+      <c r="Y16" s="60">
+        <f t="shared" si="9"/>
         <v>42946</v>
       </c>
-      <c r="Z16" s="62" t="s">
+      <c r="Z16" s="61" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5516,65 +5601,65 @@
       <c r="J17" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="60">
-        <f t="shared" ref="K17:K18" si="10">MAX($Q$16:$Q$18)/SUBTOTAL(102,$Q$16:$Q$18)</f>
-        <v>0.84</v>
-      </c>
-      <c r="L17" s="58">
+      <c r="K17" s="58">
         <f>D17-408</f>
         <v>292</v>
       </c>
-      <c r="M17" s="58">
+      <c r="L17" s="55">
+        <v>42946.734722222223</v>
+      </c>
+      <c r="M17" s="66">
         <v>300</v>
       </c>
-      <c r="N17" s="55">
-        <v>42946.734722222223</v>
+      <c r="N17" s="69">
+        <f t="shared" ref="N17:N18" si="19">MAX($Q$16:$Q$18)/SUBTOTAL(102,$Q$16:$Q$18)</f>
+        <v>0.84</v>
       </c>
       <c r="O17" s="48">
-        <f>M17-D17</f>
+        <f t="shared" si="12"/>
         <v>-400</v>
       </c>
       <c r="P17" s="49">
-        <f>IF(L17&gt;D17,INT((L17-D17)*0.95),L17-D17)</f>
+        <f t="shared" si="0"/>
         <v>-408</v>
       </c>
       <c r="Q17" s="50">
-        <f>ROUND((N17-A17)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.38</v>
       </c>
       <c r="R17" s="50">
-        <f>G17-E17</f>
+        <f t="shared" si="2"/>
         <v>153</v>
       </c>
       <c r="S17" s="50">
-        <f t="shared" ref="S17:S18" si="11">U17-T17</f>
+        <f t="shared" ref="S17:S18" si="20">U17-T17</f>
         <v>44</v>
       </c>
       <c r="T17" s="50">
-        <f>INT(E17*F17)</f>
+        <f t="shared" si="4"/>
         <v>1320</v>
       </c>
       <c r="U17" s="50">
-        <f>INT(G17*H17)</f>
+        <f t="shared" si="5"/>
         <v>1364</v>
       </c>
       <c r="V17" s="51">
+        <f t="shared" si="18"/>
+        <v>0.28758169934640521</v>
+      </c>
+      <c r="W17" s="52">
+        <f t="shared" si="7"/>
+        <v>-66.666666666666657</v>
+      </c>
+      <c r="X17" s="52">
+        <f t="shared" si="8"/>
+        <v>-42.857142857142861</v>
+      </c>
+      <c r="Y17" s="60">
         <f t="shared" si="9"/>
-        <v>0.28758169934640521</v>
-      </c>
-      <c r="W17" s="52">
-        <f>P17/R17*100/I17</f>
-        <v>-66.666666666666657</v>
-      </c>
-      <c r="X17" s="52">
-        <f>P17/Q17/I17</f>
-        <v>-42.857142857142861</v>
-      </c>
-      <c r="Y17" s="61">
-        <f>DATE(YEAR(A17),MONTH(A17),DAY(A17))</f>
         <v>42946</v>
       </c>
-      <c r="Z17" s="62" t="s">
+      <c r="Z17" s="61" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5610,64 +5695,64 @@
       <c r="J18" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="K18" s="60">
-        <f t="shared" si="10"/>
+      <c r="K18" s="58">
+        <v>519</v>
+      </c>
+      <c r="L18" s="55">
+        <v>42946.745138888888</v>
+      </c>
+      <c r="M18" s="66">
+        <v>519</v>
+      </c>
+      <c r="N18" s="69">
+        <f t="shared" si="19"/>
         <v>0.84</v>
       </c>
-      <c r="L18" s="58">
-        <v>519</v>
-      </c>
-      <c r="M18" s="58">
-        <v>519</v>
-      </c>
-      <c r="N18" s="55">
-        <v>42946.745138888888</v>
-      </c>
       <c r="O18" s="48">
-        <f>M18-D18</f>
+        <f t="shared" si="12"/>
         <v>119</v>
       </c>
       <c r="P18" s="49">
-        <f>IF(L18&gt;D18,INT((L18-D18)*0.95),L18-D18)</f>
+        <f t="shared" si="0"/>
         <v>113</v>
       </c>
       <c r="Q18" s="50">
-        <f>ROUND((N18-A18)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>1.62</v>
       </c>
       <c r="R18" s="50">
-        <f>G18-E18</f>
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="S18" s="50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>37</v>
       </c>
       <c r="T18" s="50">
-        <f>INT(E18*F18)</f>
+        <f t="shared" si="4"/>
         <v>1713</v>
       </c>
       <c r="U18" s="50">
-        <f>INT(G18*H18)</f>
+        <f t="shared" si="5"/>
         <v>1750</v>
       </c>
       <c r="V18" s="51">
+        <f t="shared" si="18"/>
+        <v>0.34905660377358488</v>
+      </c>
+      <c r="W18" s="52">
+        <f t="shared" si="7"/>
+        <v>26.650943396226417</v>
+      </c>
+      <c r="X18" s="52">
+        <f t="shared" si="8"/>
+        <v>17.438271604938272</v>
+      </c>
+      <c r="Y18" s="60">
         <f t="shared" si="9"/>
-        <v>0.34905660377358488</v>
-      </c>
-      <c r="W18" s="52">
-        <f>P18/R18*100/I18</f>
-        <v>26.650943396226417</v>
-      </c>
-      <c r="X18" s="52">
-        <f>P18/Q18/I18</f>
-        <v>17.438271604938272</v>
-      </c>
-      <c r="Y18" s="61">
-        <f>DATE(YEAR(A18),MONTH(A18),DAY(A18))</f>
         <v>42946</v>
       </c>
-      <c r="Z18" s="62" t="s">
+      <c r="Z18" s="61" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5685,80 +5770,80 @@
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="E19" s="68">
+      <c r="E19" s="67">
         <v>2997</v>
       </c>
-      <c r="F19" s="68">
+      <c r="F19" s="67">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G19" s="68">
+      <c r="G19" s="67">
         <v>3686</v>
       </c>
-      <c r="H19" s="68">
+      <c r="H19" s="67">
         <v>0.56999999999999995</v>
       </c>
-      <c r="I19" s="68">
+      <c r="I19" s="67">
         <v>4</v>
       </c>
-      <c r="J19" s="69" t="s">
+      <c r="J19" s="68" t="s">
         <v>222</v>
       </c>
-      <c r="K19" s="70">
+      <c r="K19" s="46">
+        <f>D19+111</f>
+        <v>511</v>
+      </c>
+      <c r="L19" s="47">
+        <v>42946.927777777775</v>
+      </c>
+      <c r="M19" s="66">
+        <v>508</v>
+      </c>
+      <c r="N19" s="69">
         <f>MAX($Q$19:$Q$21)/SUBTOTAL(102,$Q$19:$Q$21)</f>
         <v>0.86</v>
       </c>
-      <c r="L19" s="46">
-        <f>D19+111</f>
-        <v>511</v>
-      </c>
-      <c r="M19" s="67">
-        <v>508</v>
-      </c>
-      <c r="N19" s="47">
-        <v>42946.927777777775</v>
-      </c>
       <c r="O19" s="48">
-        <f>M19-D19</f>
+        <f t="shared" si="12"/>
         <v>108</v>
       </c>
       <c r="P19" s="49">
-        <f>IF(L19&gt;D19,INT((L19-D19)*0.95),L19-D19)</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
       <c r="Q19" s="50">
-        <f>ROUND((N19-A19)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.52</v>
       </c>
       <c r="R19" s="50">
-        <f>G19-E19</f>
+        <f t="shared" si="2"/>
         <v>689</v>
       </c>
       <c r="S19" s="50">
-        <f t="shared" ref="S19:S22" si="12">U19-T19</f>
+        <f t="shared" ref="S19:S22" si="21">U19-T19</f>
         <v>453</v>
       </c>
       <c r="T19" s="50">
-        <f>INT(E19*F19)</f>
+        <f t="shared" si="4"/>
         <v>1648</v>
       </c>
       <c r="U19" s="50">
-        <f>INT(G19*H19)</f>
+        <f t="shared" si="5"/>
         <v>2101</v>
       </c>
       <c r="V19" s="51">
-        <f t="shared" ref="V19:V22" si="13">S19/R19</f>
+        <f t="shared" ref="V19:V22" si="22">S19/R19</f>
         <v>0.65747460087082732</v>
       </c>
       <c r="W19" s="52">
-        <f>P19/R19*100/I19</f>
+        <f t="shared" si="7"/>
         <v>3.8098693759071116</v>
       </c>
       <c r="X19" s="52">
-        <f>P19/Q19/I19</f>
+        <f t="shared" si="8"/>
         <v>10.416666666666666</v>
       </c>
       <c r="Y19" s="53">
-        <f>DATE(YEAR(A19),MONTH(A19),DAY(A19))</f>
+        <f t="shared" si="9"/>
         <v>42946</v>
       </c>
       <c r="Z19" s="54" t="s">
@@ -5779,80 +5864,80 @@
         <f>400+400</f>
         <v>800</v>
       </c>
-      <c r="E20" s="68">
+      <c r="E20" s="67">
         <v>1994</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="67">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G20" s="68">
+      <c r="G20" s="67">
         <v>2497</v>
       </c>
-      <c r="H20" s="68">
+      <c r="H20" s="67">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I20" s="68">
+      <c r="I20" s="67">
         <v>4</v>
       </c>
-      <c r="J20" s="69" t="s">
+      <c r="J20" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="K20" s="70">
-        <f t="shared" ref="K20:K21" si="14">MAX($Q$19:$Q$21)/SUBTOTAL(102,$Q$19:$Q$21)</f>
-        <v>0.86</v>
-      </c>
-      <c r="L20" s="46">
+      <c r="K20" s="46">
         <f>D20-256</f>
         <v>544</v>
       </c>
-      <c r="M20" s="67">
+      <c r="L20" s="47">
+        <v>42946.945833333331</v>
+      </c>
+      <c r="M20" s="66">
         <v>560</v>
       </c>
-      <c r="N20" s="47">
-        <v>42946.945833333331</v>
+      <c r="N20" s="69">
+        <f t="shared" ref="N20:N21" si="23">MAX($Q$19:$Q$21)/SUBTOTAL(102,$Q$19:$Q$21)</f>
+        <v>0.86</v>
       </c>
       <c r="O20" s="48">
-        <f>M20-D20</f>
+        <f t="shared" si="12"/>
         <v>-240</v>
       </c>
       <c r="P20" s="49">
-        <f>IF(L20&gt;D20,INT((L20-D20)*0.95),L20-D20)</f>
+        <f t="shared" si="0"/>
         <v>-256</v>
       </c>
       <c r="Q20" s="50">
-        <f>ROUND((N20-A20)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.5299999999999998</v>
       </c>
       <c r="R20" s="50">
-        <f>G20-E20</f>
+        <f t="shared" si="2"/>
         <v>503</v>
       </c>
       <c r="S20" s="50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>282</v>
       </c>
       <c r="T20" s="50">
-        <f>INT(E20*F20)</f>
+        <f t="shared" si="4"/>
         <v>1116</v>
       </c>
       <c r="U20" s="50">
-        <f>INT(G20*H20)</f>
+        <f t="shared" si="5"/>
         <v>1398</v>
       </c>
       <c r="V20" s="51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>0.56063618290258455</v>
       </c>
       <c r="W20" s="52">
-        <f>P20/R20*100/I20</f>
+        <f t="shared" si="7"/>
         <v>-12.72365805168986</v>
       </c>
       <c r="X20" s="52">
-        <f>P20/Q20/I20</f>
+        <f t="shared" si="8"/>
         <v>-25.296442687747039</v>
       </c>
       <c r="Y20" s="53">
-        <f>DATE(YEAR(A20),MONTH(A20),DAY(A20))</f>
+        <f t="shared" si="9"/>
         <v>42946</v>
       </c>
       <c r="Z20" s="54" t="s">
@@ -5873,80 +5958,80 @@
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="E21" s="68">
+      <c r="E21" s="67">
         <v>2557</v>
       </c>
-      <c r="F21" s="68">
+      <c r="F21" s="67">
         <v>0.59</v>
       </c>
-      <c r="G21" s="68">
+      <c r="G21" s="67">
         <v>3015</v>
       </c>
-      <c r="H21" s="68">
+      <c r="H21" s="67">
         <v>0.59</v>
       </c>
-      <c r="I21" s="68">
+      <c r="I21" s="67">
         <v>4</v>
       </c>
-      <c r="J21" s="69" t="s">
+      <c r="J21" s="68" t="s">
         <v>224</v>
       </c>
-      <c r="K21" s="70">
-        <f t="shared" si="14"/>
-        <v>0.86</v>
-      </c>
-      <c r="L21" s="46">
+      <c r="K21" s="46">
         <f>D21+499</f>
         <v>899</v>
       </c>
-      <c r="M21" s="67">
+      <c r="L21" s="47">
+        <v>42946.90625</v>
+      </c>
+      <c r="M21" s="66">
         <v>884</v>
       </c>
-      <c r="N21" s="47">
-        <v>42946.90625</v>
+      <c r="N21" s="69">
+        <f t="shared" si="23"/>
+        <v>0.86</v>
       </c>
       <c r="O21" s="48">
-        <f>M21-D21</f>
+        <f t="shared" si="12"/>
         <v>484</v>
       </c>
       <c r="P21" s="49">
-        <f>IF(L21&gt;D21,INT((L21-D21)*0.95),L21-D21)</f>
+        <f t="shared" si="0"/>
         <v>474</v>
       </c>
       <c r="Q21" s="50">
-        <f>ROUND((N21-A21)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.58</v>
       </c>
       <c r="R21" s="50">
-        <f>G21-E21</f>
+        <f t="shared" si="2"/>
         <v>458</v>
       </c>
       <c r="S21" s="50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>270</v>
       </c>
       <c r="T21" s="50">
-        <f>INT(E21*F21)</f>
+        <f t="shared" si="4"/>
         <v>1508</v>
       </c>
       <c r="U21" s="50">
-        <f>INT(G21*H21)</f>
+        <f t="shared" si="5"/>
         <v>1778</v>
       </c>
       <c r="V21" s="51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>0.58951965065502188</v>
       </c>
       <c r="W21" s="52">
-        <f>P21/R21*100/I21</f>
+        <f t="shared" si="7"/>
         <v>25.873362445414848</v>
       </c>
       <c r="X21" s="52">
-        <f>P21/Q21/I21</f>
+        <f t="shared" si="8"/>
         <v>45.930232558139537</v>
       </c>
       <c r="Y21" s="53">
-        <f>DATE(YEAR(A21),MONTH(A21),DAY(A21))</f>
+        <f t="shared" si="9"/>
         <v>42946</v>
       </c>
       <c r="Z21" s="54" t="s">
@@ -5984,65 +6069,65 @@
       <c r="J22" s="59" t="s">
         <v>363</v>
       </c>
-      <c r="K22" s="60">
+      <c r="K22" s="58">
+        <f>D22-125</f>
+        <v>275</v>
+      </c>
+      <c r="L22" s="55">
+        <v>42954.978472222225</v>
+      </c>
+      <c r="M22" s="66">
+        <v>275</v>
+      </c>
+      <c r="N22" s="69">
         <f>MAX($Q$22:$Q$25)/SUBTOTAL(102,$Q$22:$Q$25)</f>
         <v>0.40500000000000003</v>
       </c>
-      <c r="L22" s="58">
-        <f>D22-125</f>
-        <v>275</v>
-      </c>
-      <c r="M22" s="58">
-        <v>275</v>
-      </c>
-      <c r="N22" s="55">
-        <v>42954.978472222225</v>
-      </c>
       <c r="O22" s="48">
-        <f>M22-D22</f>
+        <f t="shared" si="12"/>
         <v>-125</v>
       </c>
       <c r="P22" s="49">
-        <f>IF(L22&gt;D22,INT((L22-D22)*0.95),L22-D22)</f>
+        <f t="shared" si="0"/>
         <v>-125</v>
       </c>
       <c r="Q22" s="50">
-        <f>ROUND((N22-A22)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>1.62</v>
       </c>
       <c r="R22" s="50">
-        <f>G22-E22</f>
+        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="S22" s="50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
       <c r="T22" s="50">
-        <f>INT(E22*F22)</f>
+        <f t="shared" si="4"/>
         <v>1833</v>
       </c>
       <c r="U22" s="50">
-        <f>INT(G22*H22)</f>
+        <f t="shared" si="5"/>
         <v>1837</v>
       </c>
       <c r="V22" s="51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>4.0816326530612242E-2</v>
       </c>
       <c r="W22" s="52">
-        <f>P22/R22*100/I22</f>
+        <f t="shared" si="7"/>
         <v>-31.887755102040817</v>
       </c>
       <c r="X22" s="52">
-        <f>P22/Q22/I22</f>
+        <f t="shared" si="8"/>
         <v>-19.290123456790123</v>
       </c>
-      <c r="Y22" s="61">
-        <f>DATE(YEAR(A22),MONTH(A22),DAY(A22))</f>
+      <c r="Y22" s="60">
+        <f t="shared" si="9"/>
         <v>42954</v>
       </c>
-      <c r="Z22" s="62" t="s">
+      <c r="Z22" s="61" t="s">
         <v>364</v>
       </c>
     </row>
@@ -6077,65 +6162,65 @@
       <c r="J23" s="59" t="s">
         <v>367</v>
       </c>
-      <c r="K23" s="60">
-        <f t="shared" ref="K23:K25" si="15">MAX($Q$22:$Q$25)/SUBTOTAL(102,$Q$22:$Q$25)</f>
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="L23" s="58">
+      <c r="K23" s="58">
         <f>D23-62</f>
         <v>138</v>
       </c>
-      <c r="M23" s="58">
+      <c r="L23" s="55">
+        <v>42954.978472222225</v>
+      </c>
+      <c r="M23" s="66">
         <v>138</v>
       </c>
-      <c r="N23" s="55">
-        <v>42954.978472222225</v>
+      <c r="N23" s="69">
+        <f t="shared" ref="N23:N25" si="24">MAX($Q$22:$Q$25)/SUBTOTAL(102,$Q$22:$Q$25)</f>
+        <v>0.40500000000000003</v>
       </c>
       <c r="O23" s="48">
-        <f>M23-D23</f>
+        <f t="shared" si="12"/>
         <v>-62</v>
       </c>
       <c r="P23" s="49">
-        <f>IF(L23&gt;D23,INT((L23-D23)*0.95),L23-D23)</f>
+        <f t="shared" si="0"/>
         <v>-62</v>
       </c>
       <c r="Q23" s="50">
-        <f>ROUND((N23-A23)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="R23" s="50">
-        <f>G23-E23</f>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="S23" s="50">
-        <f t="shared" ref="S23:S25" si="16">U23-T23</f>
+        <f t="shared" ref="S23:S25" si="25">U23-T23</f>
         <v>13</v>
       </c>
       <c r="T23" s="50">
-        <f>INT(E23*F23)</f>
+        <f t="shared" si="4"/>
         <v>2391</v>
       </c>
       <c r="U23" s="50">
-        <f>INT(G23*H23)</f>
+        <f t="shared" si="5"/>
         <v>2404</v>
       </c>
       <c r="V23" s="51">
-        <f t="shared" ref="V23:V25" si="17">S23/R23</f>
+        <f t="shared" ref="V23:V25" si="26">S23/R23</f>
         <v>0.14444444444444443</v>
       </c>
       <c r="W23" s="52">
-        <f>P23/R23*100/I23</f>
+        <f t="shared" si="7"/>
         <v>-34.444444444444443</v>
       </c>
       <c r="X23" s="52">
-        <f>P23/Q23/I23</f>
+        <f t="shared" si="8"/>
         <v>-20.666666666666668</v>
       </c>
-      <c r="Y23" s="61">
-        <f>DATE(YEAR(A23),MONTH(A23),DAY(A23))</f>
+      <c r="Y23" s="60">
+        <f t="shared" si="9"/>
         <v>42954</v>
       </c>
-      <c r="Z23" s="62" t="s">
+      <c r="Z23" s="61" t="s">
         <v>368</v>
       </c>
     </row>
@@ -6170,65 +6255,65 @@
       <c r="J24" s="59" t="s">
         <v>371</v>
       </c>
-      <c r="K24" s="60">
-        <f t="shared" si="15"/>
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="L24" s="58">
+      <c r="K24" s="58">
         <f>D24+238</f>
         <v>638</v>
       </c>
-      <c r="M24" s="58">
+      <c r="L24" s="55">
+        <v>42954.978472222225</v>
+      </c>
+      <c r="M24" s="66">
         <v>638</v>
       </c>
-      <c r="N24" s="55">
-        <v>42954.978472222225</v>
+      <c r="N24" s="69">
+        <f t="shared" si="24"/>
+        <v>0.40500000000000003</v>
       </c>
       <c r="O24" s="48">
-        <f>M24-D24</f>
+        <f t="shared" si="12"/>
         <v>238</v>
       </c>
       <c r="P24" s="49">
-        <f>IF(L24&gt;D24,INT((L24-D24)*0.95),L24-D24)</f>
+        <f t="shared" si="0"/>
         <v>226</v>
       </c>
       <c r="Q24" s="50">
-        <f>ROUND((N24-A24)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="R24" s="50">
-        <f>G24-E24</f>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="S24" s="50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>28</v>
       </c>
       <c r="T24" s="50">
-        <f>INT(E24*F24)</f>
+        <f t="shared" si="4"/>
         <v>1897</v>
       </c>
       <c r="U24" s="50">
-        <f>INT(G24*H24)</f>
+        <f t="shared" si="5"/>
         <v>1925</v>
       </c>
       <c r="V24" s="51">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>0.30107526881720431</v>
       </c>
       <c r="W24" s="52">
-        <f>P24/R24*100/I24</f>
+        <f t="shared" si="7"/>
         <v>60.752688172043015</v>
       </c>
       <c r="X24" s="52">
-        <f>P24/Q24/I24</f>
+        <f t="shared" si="8"/>
         <v>37.666666666666664</v>
       </c>
-      <c r="Y24" s="61">
-        <f>DATE(YEAR(A24),MONTH(A24),DAY(A24))</f>
+      <c r="Y24" s="60">
+        <f t="shared" si="9"/>
         <v>42954</v>
       </c>
-      <c r="Z24" s="62" t="s">
+      <c r="Z24" s="61" t="s">
         <v>372</v>
       </c>
     </row>
@@ -6263,65 +6348,65 @@
       <c r="J25" s="59" t="s">
         <v>375</v>
       </c>
-      <c r="K25" s="60">
-        <f t="shared" si="15"/>
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="L25" s="58">
+      <c r="K25" s="58">
         <f>D25+74</f>
         <v>274</v>
       </c>
-      <c r="M25" s="58">
+      <c r="L25" s="55">
+        <v>42954.978472222225</v>
+      </c>
+      <c r="M25" s="66">
         <v>270</v>
       </c>
-      <c r="N25" s="55">
-        <v>42954.978472222225</v>
+      <c r="N25" s="69">
+        <f t="shared" si="24"/>
+        <v>0.40500000000000003</v>
       </c>
       <c r="O25" s="48">
-        <f>M25-D25</f>
+        <f t="shared" si="12"/>
         <v>70</v>
       </c>
       <c r="P25" s="49">
-        <f>IF(L25&gt;D25,INT((L25-D25)*0.95),L25-D25)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="Q25" s="50">
-        <f>ROUND((N25-A25)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>1.47</v>
       </c>
       <c r="R25" s="50">
-        <f>G25-E25</f>
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="S25" s="50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>17</v>
       </c>
       <c r="T25" s="50">
-        <f>INT(E25*F25)</f>
+        <f t="shared" si="4"/>
         <v>2227</v>
       </c>
       <c r="U25" s="50">
-        <f>INT(G25*H25)</f>
+        <f t="shared" si="5"/>
         <v>2244</v>
       </c>
       <c r="V25" s="51">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>0.2073170731707317</v>
       </c>
       <c r="W25" s="52">
-        <f>P25/R25*100/I25</f>
+        <f t="shared" si="7"/>
         <v>42.68292682926829</v>
       </c>
       <c r="X25" s="52">
-        <f>P25/Q25/I25</f>
+        <f t="shared" si="8"/>
         <v>23.80952380952381</v>
       </c>
-      <c r="Y25" s="61">
-        <f>DATE(YEAR(A25),MONTH(A25),DAY(A25))</f>
+      <c r="Y25" s="60">
+        <f t="shared" si="9"/>
         <v>42954</v>
       </c>
-      <c r="Z25" s="62" t="s">
+      <c r="Z25" s="61" t="s">
         <v>376</v>
       </c>
     </row>
@@ -6339,49 +6424,52 @@
         <f>200+400</f>
         <v>600</v>
       </c>
-      <c r="E26" s="68">
+      <c r="E26" s="67">
         <v>3177</v>
       </c>
-      <c r="F26" s="68">
+      <c r="F26" s="67">
         <v>0.65</v>
       </c>
-      <c r="G26" s="68">
+      <c r="G26" s="67">
         <v>3294</v>
       </c>
-      <c r="H26" s="68">
+      <c r="H26" s="67">
         <v>0.63</v>
       </c>
-      <c r="I26" s="68">
+      <c r="I26" s="67">
         <v>4</v>
       </c>
-      <c r="J26" s="69" t="s">
+      <c r="J26" s="68" t="s">
         <v>399</v>
       </c>
-      <c r="K26" s="70">
+      <c r="K26" s="46">
+        <f>D26+322</f>
+        <v>922</v>
+      </c>
+      <c r="L26" s="47">
+        <v>42958.033333333333</v>
+      </c>
+      <c r="M26" s="66">
+        <v>905</v>
+      </c>
+      <c r="N26" s="69">
         <f>MAX($Q$26:$Q$29)/SUBTOTAL(102,$Q$26:$Q$29)</f>
         <v>0.62</v>
       </c>
-      <c r="L26" s="46">
-        <f>D26+322</f>
-        <v>922</v>
-      </c>
-      <c r="N26" s="47">
-        <v>42958.033333333333</v>
-      </c>
       <c r="O26" s="48">
-        <f>M26-D26</f>
-        <v>-600</v>
+        <f t="shared" si="12"/>
+        <v>305</v>
       </c>
       <c r="P26" s="49">
-        <f>IF(L26&gt;D26,INT((L26-D26)*0.95),L26-D26)</f>
+        <f t="shared" si="0"/>
         <v>305</v>
       </c>
       <c r="Q26" s="50">
-        <f>ROUND((N26-A26)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>1.93</v>
       </c>
       <c r="R26" s="50">
-        <f>G26-E26</f>
+        <f t="shared" si="2"/>
         <v>117</v>
       </c>
       <c r="S26" s="50">
@@ -6389,11 +6477,11 @@
         <v>10</v>
       </c>
       <c r="T26" s="50">
-        <f>INT(E26*F26)</f>
+        <f t="shared" si="4"/>
         <v>2065</v>
       </c>
       <c r="U26" s="50">
-        <f>INT(G26*H26)</f>
+        <f t="shared" si="5"/>
         <v>2075</v>
       </c>
       <c r="V26" s="51">
@@ -6401,15 +6489,15 @@
         <v>8.5470085470085472E-2</v>
       </c>
       <c r="W26" s="52">
-        <f>P26/R26*100/I26</f>
+        <f t="shared" si="7"/>
         <v>65.17094017094017</v>
       </c>
       <c r="X26" s="52">
-        <f>P26/Q26/I26</f>
+        <f t="shared" si="8"/>
         <v>39.50777202072539</v>
       </c>
       <c r="Y26" s="53">
-        <f>DATE(YEAR(A26),MONTH(A26),DAY(A26))</f>
+        <f t="shared" si="9"/>
         <v>42957</v>
       </c>
       <c r="Z26" s="54" t="s">
@@ -6430,61 +6518,64 @@
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="E27" s="68">
+      <c r="E27" s="67">
         <v>4420</v>
       </c>
-      <c r="F27" s="68">
+      <c r="F27" s="67">
         <v>0.62</v>
       </c>
-      <c r="G27" s="68">
+      <c r="G27" s="67">
         <v>4580</v>
       </c>
-      <c r="H27" s="68">
+      <c r="H27" s="67">
         <v>0.61</v>
       </c>
-      <c r="I27" s="68">
+      <c r="I27" s="67">
         <v>4</v>
       </c>
-      <c r="J27" s="69" t="s">
+      <c r="J27" s="68" t="s">
         <v>399</v>
       </c>
-      <c r="K27" s="70">
-        <f t="shared" ref="K27:K29" si="18">MAX($Q$26:$Q$29)/SUBTOTAL(102,$Q$26:$Q$29)</f>
-        <v>0.62</v>
-      </c>
-      <c r="L27" s="46">
+      <c r="K27" s="46">
         <f>D27+256</f>
         <v>656</v>
       </c>
-      <c r="N27" s="47">
+      <c r="L27" s="47">
         <v>42958.033333333333</v>
       </c>
+      <c r="M27" s="66">
+        <v>648</v>
+      </c>
+      <c r="N27" s="69">
+        <f t="shared" ref="N27:N29" si="27">MAX($Q$26:$Q$29)/SUBTOTAL(102,$Q$26:$Q$29)</f>
+        <v>0.62</v>
+      </c>
       <c r="O27" s="48">
-        <f>M27-D27</f>
-        <v>-400</v>
+        <f t="shared" si="12"/>
+        <v>248</v>
       </c>
       <c r="P27" s="49">
-        <f>IF(L27&gt;D27,INT((L27-D27)*0.95),L27-D27)</f>
+        <f t="shared" si="0"/>
         <v>243</v>
       </c>
       <c r="Q27" s="50">
-        <f>ROUND((N27-A27)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.48</v>
       </c>
       <c r="R27" s="50">
-        <f>G27-E27</f>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="S27" s="50">
-        <f t="shared" ref="S27:S29" si="19">U27-T27</f>
+        <f t="shared" ref="S27:S33" si="28">U27-T27</f>
         <v>53</v>
       </c>
       <c r="T27" s="50">
-        <f>INT(E27*F27)</f>
+        <f t="shared" si="4"/>
         <v>2740</v>
       </c>
       <c r="U27" s="50">
-        <f>INT(G27*H27)</f>
+        <f t="shared" si="5"/>
         <v>2793</v>
       </c>
       <c r="V27" s="51">
@@ -6492,15 +6583,15 @@
         <v>0.33124999999999999</v>
       </c>
       <c r="W27" s="52">
-        <f>P27/R27*100/I27</f>
+        <f t="shared" si="7"/>
         <v>37.96875</v>
       </c>
       <c r="X27" s="52">
-        <f>P27/Q27/I27</f>
+        <f t="shared" si="8"/>
         <v>24.495967741935484</v>
       </c>
       <c r="Y27" s="53">
-        <f>DATE(YEAR(A27),MONTH(A27),DAY(A27))</f>
+        <f t="shared" si="9"/>
         <v>42957</v>
       </c>
       <c r="Z27" s="54" t="s">
@@ -6521,49 +6612,52 @@
         <f>400</f>
         <v>400</v>
       </c>
-      <c r="E28" s="68">
+      <c r="E28" s="67">
         <v>3244</v>
       </c>
-      <c r="F28" s="68">
+      <c r="F28" s="67">
         <v>0.64</v>
       </c>
-      <c r="G28" s="68">
+      <c r="G28" s="67">
         <v>3341</v>
       </c>
-      <c r="H28" s="68">
+      <c r="H28" s="67">
         <v>0.624</v>
       </c>
-      <c r="I28" s="68">
+      <c r="I28" s="67">
         <v>4</v>
       </c>
-      <c r="J28" s="69" t="s">
+      <c r="J28" s="68" t="s">
         <v>399</v>
       </c>
-      <c r="K28" s="70">
-        <f t="shared" si="18"/>
-        <v>0.62</v>
-      </c>
-      <c r="L28" s="46">
+      <c r="K28" s="46">
         <f>D28-19</f>
         <v>381</v>
       </c>
-      <c r="N28" s="47">
+      <c r="L28" s="47">
         <v>42958.033333333333</v>
       </c>
+      <c r="M28" s="66">
+        <v>381</v>
+      </c>
+      <c r="N28" s="69">
+        <f t="shared" si="27"/>
+        <v>0.62</v>
+      </c>
       <c r="O28" s="48">
-        <f>M28-D28</f>
-        <v>-400</v>
+        <f t="shared" si="12"/>
+        <v>-19</v>
       </c>
       <c r="P28" s="49">
-        <f>IF(L28&gt;D28,INT((L28-D28)*0.95),L28-D28)</f>
+        <f t="shared" si="0"/>
         <v>-19</v>
       </c>
       <c r="Q28" s="50">
-        <f>ROUND((N28-A28)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>1.35</v>
       </c>
       <c r="R28" s="50">
-        <f>G28-E28</f>
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
       <c r="S28" s="50">
@@ -6571,11 +6665,11 @@
         <v>8</v>
       </c>
       <c r="T28" s="50">
-        <f>INT(E28*F28)</f>
+        <f t="shared" si="4"/>
         <v>2076</v>
       </c>
       <c r="U28" s="50">
-        <f>INT(G28*H28)</f>
+        <f t="shared" si="5"/>
         <v>2084</v>
       </c>
       <c r="V28" s="51">
@@ -6583,15 +6677,15 @@
         <v>8.247422680412371E-2</v>
       </c>
       <c r="W28" s="52">
-        <f>P28/R28*100/I28</f>
+        <f t="shared" si="7"/>
         <v>-4.8969072164948457</v>
       </c>
       <c r="X28" s="52">
-        <f>P28/Q28/I28</f>
+        <f t="shared" si="8"/>
         <v>-3.5185185185185182</v>
       </c>
       <c r="Y28" s="53">
-        <f>DATE(YEAR(A28),MONTH(A28),DAY(A28))</f>
+        <f t="shared" si="9"/>
         <v>42957</v>
       </c>
       <c r="Z28" s="54" t="s">
@@ -6612,81 +6706,707 @@
         <f>400+200</f>
         <v>600</v>
       </c>
-      <c r="E29" s="68">
+      <c r="E29" s="67">
         <v>3562</v>
       </c>
-      <c r="F29" s="68">
+      <c r="F29" s="67">
         <v>0.63</v>
       </c>
-      <c r="G29" s="68">
+      <c r="G29" s="67">
         <v>3726</v>
       </c>
-      <c r="H29" s="68">
+      <c r="H29" s="67">
         <v>0.61</v>
       </c>
-      <c r="I29" s="68">
+      <c r="I29" s="67">
         <v>4</v>
       </c>
-      <c r="J29" s="69" t="s">
+      <c r="J29" s="68" t="s">
         <v>398</v>
       </c>
-      <c r="K29" s="70">
-        <f t="shared" si="18"/>
-        <v>0.62</v>
-      </c>
-      <c r="L29" s="46">
+      <c r="K29" s="46">
         <f>D29-208</f>
         <v>392</v>
       </c>
-      <c r="N29" s="47">
+      <c r="L29" s="47">
         <v>42958.033333333333</v>
       </c>
+      <c r="M29" s="66">
+        <v>392</v>
+      </c>
+      <c r="N29" s="69">
+        <f t="shared" si="27"/>
+        <v>0.62</v>
+      </c>
       <c r="O29" s="48">
-        <f>M29-D29</f>
-        <v>-600</v>
+        <f t="shared" si="12"/>
+        <v>-208</v>
       </c>
       <c r="P29" s="49">
-        <f>IF(L29&gt;D29,INT((L29-D29)*0.95),L29-D29)</f>
+        <f t="shared" si="0"/>
         <v>-208</v>
       </c>
       <c r="Q29" s="50">
-        <f>ROUND((N29-A29)*24,2)</f>
+        <f t="shared" si="1"/>
         <v>2.42</v>
       </c>
       <c r="R29" s="50">
-        <f>G29-E29</f>
+        <f t="shared" si="2"/>
         <v>164</v>
       </c>
       <c r="S29" s="50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>28</v>
       </c>
       <c r="T29" s="50">
-        <f>INT(E29*F29)</f>
+        <f t="shared" si="4"/>
         <v>2244</v>
       </c>
       <c r="U29" s="50">
-        <f>INT(G29*H29)</f>
+        <f t="shared" si="5"/>
         <v>2272</v>
       </c>
       <c r="V29" s="51">
-        <f t="shared" ref="V27:V29" si="20">S29/R29</f>
+        <f t="shared" ref="V29:V33" si="29">S29/R29</f>
         <v>0.17073170731707318</v>
       </c>
       <c r="W29" s="52">
-        <f>P29/R29*100/I29</f>
+        <f t="shared" si="7"/>
         <v>-31.707317073170731</v>
       </c>
       <c r="X29" s="52">
-        <f>P29/Q29/I29</f>
+        <f t="shared" si="8"/>
         <v>-21.487603305785125</v>
       </c>
       <c r="Y29" s="53">
-        <f>DATE(YEAR(A29),MONTH(A29),DAY(A29))</f>
+        <f t="shared" si="9"/>
         <v>42957</v>
       </c>
       <c r="Z29" s="54" t="s">
         <v>395</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" s="56" customFormat="1">
+      <c r="A30" s="55">
+        <v>42960.638194444444</v>
+      </c>
+      <c r="B30" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="57" t="s">
+        <v>406</v>
+      </c>
+      <c r="D30" s="57">
+        <f>400+200</f>
+        <v>600</v>
+      </c>
+      <c r="E30" s="57">
+        <v>3294</v>
+      </c>
+      <c r="F30" s="57">
+        <v>0.63</v>
+      </c>
+      <c r="G30" s="57">
+        <v>3442</v>
+      </c>
+      <c r="H30" s="57">
+        <v>0.61</v>
+      </c>
+      <c r="I30" s="57">
+        <v>4</v>
+      </c>
+      <c r="J30" s="59" t="s">
+        <v>409</v>
+      </c>
+      <c r="K30" s="58">
+        <f>D30-238</f>
+        <v>362</v>
+      </c>
+      <c r="L30" s="55">
+        <v>42960.725694444445</v>
+      </c>
+      <c r="M30" s="66">
+        <v>362</v>
+      </c>
+      <c r="N30" s="69">
+        <f>MAX($Q$30:$Q$33)/SUBTOTAL(102,$Q$30:$Q$33)</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O30" s="48">
+        <f t="shared" si="12"/>
+        <v>-238</v>
+      </c>
+      <c r="P30" s="49">
+        <f t="shared" si="0"/>
+        <v>-238</v>
+      </c>
+      <c r="Q30" s="50">
+        <f t="shared" si="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="R30" s="50">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="S30" s="50">
+        <f t="shared" si="28"/>
+        <v>24</v>
+      </c>
+      <c r="T30" s="50">
+        <f t="shared" si="4"/>
+        <v>2075</v>
+      </c>
+      <c r="U30" s="50">
+        <f t="shared" si="5"/>
+        <v>2099</v>
+      </c>
+      <c r="V30" s="51">
+        <f t="shared" si="29"/>
+        <v>0.16216216216216217</v>
+      </c>
+      <c r="W30" s="52">
+        <f t="shared" si="7"/>
+        <v>-40.202702702702702</v>
+      </c>
+      <c r="X30" s="52">
+        <f t="shared" si="8"/>
+        <v>-28.333333333333332</v>
+      </c>
+      <c r="Y30" s="60">
+        <f t="shared" si="9"/>
+        <v>42960</v>
+      </c>
+      <c r="Z30" s="61" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" s="56" customFormat="1">
+      <c r="A31" s="55">
+        <v>42960.638194444444</v>
+      </c>
+      <c r="B31" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="57" t="s">
+        <v>407</v>
+      </c>
+      <c r="D31" s="57">
+        <v>400</v>
+      </c>
+      <c r="E31" s="57">
+        <v>4580</v>
+      </c>
+      <c r="F31" s="57">
+        <v>0.61</v>
+      </c>
+      <c r="G31" s="57">
+        <v>4729</v>
+      </c>
+      <c r="H31" s="57">
+        <v>0.59</v>
+      </c>
+      <c r="I31" s="57">
+        <v>4</v>
+      </c>
+      <c r="J31" s="59" t="s">
+        <v>409</v>
+      </c>
+      <c r="K31" s="58">
+        <f>D31+407</f>
+        <v>807</v>
+      </c>
+      <c r="L31" s="55">
+        <v>42960.725694444445</v>
+      </c>
+      <c r="M31" s="66">
+        <v>795</v>
+      </c>
+      <c r="N31" s="69">
+        <f t="shared" ref="N31:N33" si="30">MAX($Q$30:$Q$33)/SUBTOTAL(102,$Q$30:$Q$33)</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O31" s="48">
+        <f t="shared" si="12"/>
+        <v>395</v>
+      </c>
+      <c r="P31" s="49">
+        <f t="shared" si="0"/>
+        <v>386</v>
+      </c>
+      <c r="Q31" s="50">
+        <f t="shared" si="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="R31" s="50">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+      <c r="S31" s="50">
+        <f t="shared" si="28"/>
+        <v>-3</v>
+      </c>
+      <c r="T31" s="50">
+        <f t="shared" si="4"/>
+        <v>2793</v>
+      </c>
+      <c r="U31" s="50">
+        <f t="shared" si="5"/>
+        <v>2790</v>
+      </c>
+      <c r="V31" s="51">
+        <f t="shared" si="29"/>
+        <v>-2.0134228187919462E-2</v>
+      </c>
+      <c r="W31" s="52">
+        <f t="shared" si="7"/>
+        <v>64.765100671140942</v>
+      </c>
+      <c r="X31" s="52">
+        <f t="shared" si="8"/>
+        <v>45.952380952380949</v>
+      </c>
+      <c r="Y31" s="60">
+        <f t="shared" si="9"/>
+        <v>42960</v>
+      </c>
+      <c r="Z31" s="61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" s="56" customFormat="1">
+      <c r="A32" s="55">
+        <v>42960.640972222223</v>
+      </c>
+      <c r="B32" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>408</v>
+      </c>
+      <c r="D32" s="57">
+        <v>400</v>
+      </c>
+      <c r="E32" s="57">
+        <v>3341</v>
+      </c>
+      <c r="F32" s="57">
+        <v>0.624</v>
+      </c>
+      <c r="G32" s="57">
+        <v>3461</v>
+      </c>
+      <c r="H32" s="57">
+        <v>0.61</v>
+      </c>
+      <c r="I32" s="57">
+        <v>4</v>
+      </c>
+      <c r="J32" s="59" t="s">
+        <v>409</v>
+      </c>
+      <c r="K32" s="58">
+        <f>D32+167</f>
+        <v>567</v>
+      </c>
+      <c r="L32" s="55">
+        <v>42960.725694444445</v>
+      </c>
+      <c r="M32" s="66">
+        <v>553</v>
+      </c>
+      <c r="N32" s="69">
+        <f t="shared" si="30"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O32" s="48">
+        <f t="shared" si="12"/>
+        <v>153</v>
+      </c>
+      <c r="P32" s="49">
+        <f t="shared" si="0"/>
+        <v>158</v>
+      </c>
+      <c r="Q32" s="50">
+        <f t="shared" si="1"/>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="R32" s="50">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="S32" s="50">
+        <f t="shared" si="28"/>
+        <v>27</v>
+      </c>
+      <c r="T32" s="50">
+        <f t="shared" si="4"/>
+        <v>2084</v>
+      </c>
+      <c r="U32" s="50">
+        <f t="shared" si="5"/>
+        <v>2111</v>
+      </c>
+      <c r="V32" s="51">
+        <f t="shared" si="29"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="W32" s="52">
+        <f t="shared" si="7"/>
+        <v>32.916666666666664</v>
+      </c>
+      <c r="X32" s="52">
+        <f t="shared" si="8"/>
+        <v>19.458128078817737</v>
+      </c>
+      <c r="Y32" s="60">
+        <f t="shared" si="9"/>
+        <v>42960</v>
+      </c>
+      <c r="Z32" s="61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" s="56" customFormat="1">
+      <c r="A33" s="55">
+        <v>42960.629166666666</v>
+      </c>
+      <c r="B33" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="57" t="s">
+        <v>404</v>
+      </c>
+      <c r="D33" s="57">
+        <v>200</v>
+      </c>
+      <c r="E33" s="57">
+        <v>3726</v>
+      </c>
+      <c r="F33" s="57">
+        <v>0.61</v>
+      </c>
+      <c r="G33" s="57">
+        <v>3869</v>
+      </c>
+      <c r="H33" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="I33" s="57">
+        <v>2</v>
+      </c>
+      <c r="J33" s="59" t="s">
+        <v>405</v>
+      </c>
+      <c r="K33" s="58">
+        <f>D33+172</f>
+        <v>372</v>
+      </c>
+      <c r="L33" s="55">
+        <v>42960.725694444445</v>
+      </c>
+      <c r="M33" s="66"/>
+      <c r="N33" s="69">
+        <f t="shared" si="30"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="O33" s="48">
+        <f t="shared" si="12"/>
+        <v>-200</v>
+      </c>
+      <c r="P33" s="49">
+        <f t="shared" si="0"/>
+        <v>163</v>
+      </c>
+      <c r="Q33" s="50">
+        <f t="shared" si="1"/>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="R33" s="50">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="S33" s="50">
+        <f t="shared" si="28"/>
+        <v>49</v>
+      </c>
+      <c r="T33" s="50">
+        <f t="shared" si="4"/>
+        <v>2272</v>
+      </c>
+      <c r="U33" s="50">
+        <f t="shared" si="5"/>
+        <v>2321</v>
+      </c>
+      <c r="V33" s="51">
+        <f t="shared" si="29"/>
+        <v>0.34265734265734266</v>
+      </c>
+      <c r="W33" s="52">
+        <f t="shared" si="7"/>
+        <v>56.993006993006986</v>
+      </c>
+      <c r="X33" s="52">
+        <f t="shared" si="8"/>
+        <v>35.129310344827587</v>
+      </c>
+      <c r="Y33" s="60">
+        <f t="shared" si="9"/>
+        <v>42960</v>
+      </c>
+      <c r="Z33" s="61" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26">
+      <c r="A34" s="47">
+        <v>42960</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="44"/>
+      <c r="L34" s="47">
+        <v>42962</v>
+      </c>
+      <c r="N34" s="69">
+        <f>MAX($Q$34:$Q$37)/SUBTOTAL(102,$Q$34:$Q$37)</f>
+        <v>12</v>
+      </c>
+      <c r="O34" s="48">
+        <f t="shared" ref="O34:O37" si="31">M34-D34</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="49">
+        <f t="shared" ref="P34:P37" si="32">IF(K34&gt;D34,INT((K34-D34)*0.95),K34-D34)</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="50">
+        <f t="shared" ref="Q34:Q37" si="33">ROUND((L34-A34)*24,2)</f>
+        <v>48</v>
+      </c>
+      <c r="R34" s="50">
+        <f t="shared" ref="R34:R37" si="34">G34-E34</f>
+        <v>0</v>
+      </c>
+      <c r="S34" s="50">
+        <f>U34-T34</f>
+        <v>0</v>
+      </c>
+      <c r="T34" s="50">
+        <f t="shared" ref="T34:T37" si="35">INT(E34*F34)</f>
+        <v>0</v>
+      </c>
+      <c r="U34" s="50">
+        <f t="shared" ref="U34:U37" si="36">INT(G34*H34)</f>
+        <v>0</v>
+      </c>
+      <c r="V34" s="51" t="e">
+        <f>S34/R34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W34" s="52" t="e">
+        <f t="shared" ref="W34:W37" si="37">P34/R34*100/I34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X34" s="52" t="e">
+        <f t="shared" ref="X34:X37" si="38">P34/Q34/I34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y34" s="53">
+        <f t="shared" ref="Y34:Y37" si="39">DATE(YEAR(A34),MONTH(A34),DAY(A34))</f>
+        <v>42960</v>
+      </c>
+      <c r="Z34" s="54" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26">
+      <c r="A35" s="47">
+        <v>42960</v>
+      </c>
+      <c r="B35" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="44"/>
+      <c r="L35" s="47">
+        <v>42962</v>
+      </c>
+      <c r="N35" s="69">
+        <f t="shared" ref="N35:N37" si="40">MAX($Q$34:$Q$37)/SUBTOTAL(102,$Q$34:$Q$37)</f>
+        <v>12</v>
+      </c>
+      <c r="O35" s="48">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="49">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="50">
+        <f t="shared" si="33"/>
+        <v>48</v>
+      </c>
+      <c r="R35" s="50">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S35" s="50">
+        <f t="shared" ref="S35" si="41">U35-T35</f>
+        <v>0</v>
+      </c>
+      <c r="T35" s="50">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="U35" s="50">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="V35" s="51" t="e">
+        <f>S35/R35</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W35" s="52" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X35" s="52" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y35" s="53">
+        <f t="shared" si="39"/>
+        <v>42960</v>
+      </c>
+      <c r="Z35" s="54" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26">
+      <c r="A36" s="47">
+        <v>42960</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="44"/>
+      <c r="L36" s="47">
+        <v>42962</v>
+      </c>
+      <c r="N36" s="69">
+        <f t="shared" si="40"/>
+        <v>12</v>
+      </c>
+      <c r="O36" s="48">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P36" s="49">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="50">
+        <f t="shared" si="33"/>
+        <v>48</v>
+      </c>
+      <c r="R36" s="50">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S36" s="50">
+        <f>U36-T36</f>
+        <v>0</v>
+      </c>
+      <c r="T36" s="50">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="U36" s="50">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="V36" s="51" t="e">
+        <f>S36/R36</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W36" s="52" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X36" s="52" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y36" s="53">
+        <f t="shared" si="39"/>
+        <v>42960</v>
+      </c>
+      <c r="Z36" s="54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26">
+      <c r="A37" s="47">
+        <v>42960</v>
+      </c>
+      <c r="B37" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="44"/>
+      <c r="L37" s="47">
+        <v>42962</v>
+      </c>
+      <c r="N37" s="69">
+        <f t="shared" si="40"/>
+        <v>12</v>
+      </c>
+      <c r="O37" s="48">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P37" s="49">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="50">
+        <f t="shared" si="33"/>
+        <v>48</v>
+      </c>
+      <c r="R37" s="50">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S37" s="50">
+        <f t="shared" ref="S37" si="42">U37-T37</f>
+        <v>0</v>
+      </c>
+      <c r="T37" s="50">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="U37" s="50">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="V37" s="51" t="e">
+        <f t="shared" ref="V37" si="43">S37/R37</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W37" s="52" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X37" s="52" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y37" s="53">
+        <f t="shared" si="39"/>
+        <v>42960</v>
+      </c>
+      <c r="Z37" s="54" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -7315,10 +8035,10 @@
   <dimension ref="A1:R132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -7508,7 +8228,7 @@
       <c r="J6" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="K6" s="63" t="s">
+      <c r="K6" s="62" t="s">
         <v>143</v>
       </c>
       <c r="P6" s="43" t="s">
@@ -7548,7 +8268,7 @@
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="63" t="s">
         <v>138</v>
       </c>
       <c r="D8" s="54" t="s">
@@ -7583,7 +8303,7 @@
       <c r="D9" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="F9" s="64">
+      <c r="F9" s="63">
         <v>159385</v>
       </c>
       <c r="G9" s="43" t="s">
@@ -7661,18 +8381,18 @@
       <c r="D12" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="F12" s="64">
+      <c r="F12" s="63">
         <v>180490</v>
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="63" t="s">
         <v>149</v>
       </c>
       <c r="D13" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="F13" s="64">
+      <c r="F13" s="63">
         <v>172402</v>
       </c>
       <c r="G13" s="43" t="s">
@@ -7686,7 +8406,7 @@
       <c r="D14" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="G14" s="64" t="s">
+      <c r="G14" s="63" t="s">
         <v>151</v>
       </c>
       <c r="J14" s="43" t="s">
@@ -7700,7 +8420,7 @@
       <c r="D15" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="F15" s="64">
+      <c r="F15" s="63">
         <v>136118</v>
       </c>
       <c r="J15" s="43" t="s">
@@ -7708,7 +8428,7 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="63" t="s">
         <v>153</v>
       </c>
       <c r="D16" s="54" t="s">
@@ -7719,7 +8439,7 @@
       <c r="B17" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="63" t="s">
         <v>154</v>
       </c>
       <c r="D17" s="54" t="s">
@@ -7733,7 +8453,7 @@
       <c r="D18" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="F18" s="64">
+      <c r="F18" s="63">
         <v>141928</v>
       </c>
     </row>
@@ -7761,7 +8481,7 @@
       <c r="B20" s="43" t="s">
         <v>245</v>
       </c>
-      <c r="C20" s="64" t="s">
+      <c r="C20" s="63" t="s">
         <v>161</v>
       </c>
       <c r="D20" s="54" t="s">
@@ -7784,7 +8504,7 @@
       <c r="B21" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="C21" s="63" t="s">
         <v>164</v>
       </c>
       <c r="D21" s="54" t="s">
@@ -7804,7 +8524,7 @@
       <c r="B22" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="63" t="s">
         <v>165</v>
       </c>
       <c r="D22" s="54" t="s">
@@ -7829,7 +8549,7 @@
       <c r="B24" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="64" t="s">
         <v>171</v>
       </c>
       <c r="D24" s="54" t="s">
@@ -7843,7 +8563,7 @@
       <c r="B25" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="C25" s="65" t="s">
+      <c r="C25" s="64" t="s">
         <v>173</v>
       </c>
       <c r="D25" s="54" t="s">
@@ -7854,7 +8574,7 @@
       <c r="B26" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="65">
+      <c r="C26" s="64">
         <v>13611340307</v>
       </c>
       <c r="D26" s="54" t="s">
@@ -8682,7 +9402,7 @@
       <c r="B80" s="43" t="s">
         <v>332</v>
       </c>
-      <c r="C80" s="66" t="s">
+      <c r="C80" s="65" t="s">
         <v>331</v>
       </c>
       <c r="D80" s="54" t="s">
@@ -8825,6 +9545,17 @@
       </c>
       <c r="F89" s="43">
         <v>135635</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8">
+      <c r="B90" s="43" t="s">
+        <v>402</v>
+      </c>
+      <c r="C90" s="43">
+        <v>15727929927</v>
+      </c>
+      <c r="D90" s="54" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="124" spans="2:2">

</xml_diff>

<commit_message>
modified:   view/inc/db.inc.php 	modified:   view/index.php 	modified:   view/js/func.js 	modified:   view/mdl/menu.mdl.php 	modified:   view/texas/rec_poker_self.xlsx
</commit_message>
<xml_diff>
--- a/view/texas/rec_poker_self.xlsx
+++ b/view/texas/rec_poker_self.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="755"/>
+    <workbookView xWindow="18060" yWindow="8720" windowWidth="10880" windowHeight="15200" tabRatio="755"/>
   </bookViews>
   <sheets>
     <sheet name="rec" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="417">
   <si>
     <t>user</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1797,8 +1797,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="397">
+  <cellStyleXfs count="399">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2274,7 +2276,7 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="178" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="397">
+  <cellStyles count="399">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -2473,6 +2475,7 @@
     <cellStyle name="超链接" xfId="391" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="393" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="397" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -2671,6 +2674,7 @@
     <cellStyle name="访问过的超链接" xfId="392" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="394" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="398" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
@@ -4087,13 +4091,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z37"/>
+  <dimension ref="A1:Z41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P42" sqref="P42"/>
+      <selection pane="bottomRight" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -7233,24 +7237,27 @@
       <c r="L34" s="47">
         <v>42961.958333333336</v>
       </c>
+      <c r="M34" s="66">
+        <v>469</v>
+      </c>
       <c r="N34" s="69">
         <f>MAX($Q$34:$Q$37)/SUBTOTAL(102,$Q$34:$Q$37)</f>
         <v>0.38750000000000001</v>
       </c>
       <c r="O34" s="48">
-        <f t="shared" ref="O34:O37" si="31">M34-D34</f>
-        <v>-400</v>
+        <f t="shared" ref="O34:O41" si="31">M34-D34</f>
+        <v>69</v>
       </c>
       <c r="P34" s="49">
-        <f t="shared" ref="P34:P37" si="32">IF(K34&gt;D34,INT((K34-D34)*0.95),K34-D34)</f>
+        <f t="shared" ref="P34:P41" si="32">IF(K34&gt;D34,INT((K34-D34)*0.95),K34-D34)</f>
         <v>69</v>
       </c>
       <c r="Q34" s="50">
-        <f t="shared" ref="Q34:Q37" si="33">ROUND((L34-A34)*24,2)</f>
+        <f t="shared" ref="Q34:Q41" si="33">ROUND((L34-A34)*24,2)</f>
         <v>1.1299999999999999</v>
       </c>
       <c r="R34" s="50">
-        <f t="shared" ref="R34:R37" si="34">G34-E34</f>
+        <f t="shared" ref="R34:R41" si="34">G34-E34</f>
         <v>79</v>
       </c>
       <c r="S34" s="50">
@@ -7258,11 +7265,11 @@
         <v>13</v>
       </c>
       <c r="T34" s="50">
-        <f t="shared" ref="T34:T37" si="35">INT(E34*F34)</f>
+        <f t="shared" ref="T34:T41" si="35">INT(E34*F34)</f>
         <v>2099</v>
       </c>
       <c r="U34" s="50">
-        <f t="shared" ref="U34:U37" si="36">INT(G34*H34)</f>
+        <f t="shared" ref="U34:U41" si="36">INT(G34*H34)</f>
         <v>2112</v>
       </c>
       <c r="V34" s="51">
@@ -7270,15 +7277,15 @@
         <v>0.16455696202531644</v>
       </c>
       <c r="W34" s="52">
-        <f t="shared" ref="W34:W37" si="37">P34/R34*100/I34</f>
+        <f t="shared" ref="W34:W41" si="37">P34/R34*100/I34</f>
         <v>21.835443037974684</v>
       </c>
       <c r="X34" s="52">
-        <f t="shared" ref="X34:X37" si="38">P34/Q34/I34</f>
+        <f t="shared" ref="X34:X41" si="38">P34/Q34/I34</f>
         <v>15.265486725663719</v>
       </c>
       <c r="Y34" s="53">
-        <f t="shared" ref="Y34:Y37" si="39">DATE(YEAR(A34),MONTH(A34),DAY(A34))</f>
+        <f t="shared" ref="Y34:Y41" si="39">DATE(YEAR(A34),MONTH(A34),DAY(A34))</f>
         <v>42961</v>
       </c>
       <c r="Z34" s="54" t="s">
@@ -7324,13 +7331,16 @@
       <c r="L35" s="47">
         <v>42961.958333333336</v>
       </c>
+      <c r="M35" s="66">
+        <v>166</v>
+      </c>
       <c r="N35" s="69">
         <f t="shared" ref="N35:N37" si="40">MAX($Q$34:$Q$37)/SUBTOTAL(102,$Q$34:$Q$37)</f>
         <v>0.38750000000000001</v>
       </c>
       <c r="O35" s="48">
         <f t="shared" si="31"/>
-        <v>-200</v>
+        <v>-34</v>
       </c>
       <c r="P35" s="49">
         <f t="shared" si="32"/>
@@ -7414,13 +7424,16 @@
       <c r="L36" s="47">
         <v>42961.958333333336</v>
       </c>
+      <c r="M36" s="66">
+        <v>324</v>
+      </c>
       <c r="N36" s="69">
         <f t="shared" si="40"/>
         <v>0.38750000000000001</v>
       </c>
       <c r="O36" s="48">
         <f t="shared" si="31"/>
-        <v>-200</v>
+        <v>124</v>
       </c>
       <c r="P36" s="49">
         <f t="shared" si="32"/>
@@ -7504,13 +7517,16 @@
       <c r="L37" s="47">
         <v>42961.958333333336</v>
       </c>
+      <c r="M37" s="66">
+        <v>196</v>
+      </c>
       <c r="N37" s="69">
         <f t="shared" si="40"/>
         <v>0.38750000000000001</v>
       </c>
       <c r="O37" s="48">
         <f t="shared" si="31"/>
-        <v>-200</v>
+        <v>-4</v>
       </c>
       <c r="P37" s="49">
         <f t="shared" si="32"/>
@@ -7525,7 +7541,7 @@
         <v>71</v>
       </c>
       <c r="S37" s="50">
-        <f t="shared" ref="S37" si="42">U37-T37</f>
+        <f t="shared" ref="S37:S41" si="42">U37-T37</f>
         <v>84</v>
       </c>
       <c r="T37" s="50">
@@ -7537,7 +7553,7 @@
         <v>2547</v>
       </c>
       <c r="V37" s="51">
-        <f t="shared" ref="V37" si="43">S37/R37</f>
+        <f t="shared" ref="V37:V41" si="43">S37/R37</f>
         <v>1.1830985915492958</v>
       </c>
       <c r="W37" s="52">
@@ -7553,6 +7569,310 @@
         <v>42961</v>
       </c>
       <c r="Z37" s="54" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" s="56" customFormat="1">
+      <c r="A38" s="55">
+        <v>42962</v>
+      </c>
+      <c r="B38" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57">
+        <v>3521</v>
+      </c>
+      <c r="F38" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="59"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="55">
+        <v>42964</v>
+      </c>
+      <c r="M38" s="66"/>
+      <c r="N38" s="69">
+        <f>MAX($Q$38:$Q$41)/SUBTOTAL(102,$Q$38:$Q$41)</f>
+        <v>12</v>
+      </c>
+      <c r="O38" s="48">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="49">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="50">
+        <f t="shared" si="33"/>
+        <v>48</v>
+      </c>
+      <c r="R38" s="50">
+        <f t="shared" si="34"/>
+        <v>-3521</v>
+      </c>
+      <c r="S38" s="50">
+        <f t="shared" si="42"/>
+        <v>-2112</v>
+      </c>
+      <c r="T38" s="50">
+        <f t="shared" si="35"/>
+        <v>2112</v>
+      </c>
+      <c r="U38" s="50">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="V38" s="51">
+        <f t="shared" si="43"/>
+        <v>0.59982959386537915</v>
+      </c>
+      <c r="W38" s="52" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X38" s="52" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y38" s="60">
+        <f t="shared" si="39"/>
+        <v>42962</v>
+      </c>
+      <c r="Z38" s="61" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" s="56" customFormat="1">
+      <c r="A39" s="55">
+        <v>42962</v>
+      </c>
+      <c r="B39" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57">
+        <v>5068</v>
+      </c>
+      <c r="F39" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="G39" s="57"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="57"/>
+      <c r="J39" s="59"/>
+      <c r="K39" s="58"/>
+      <c r="L39" s="55">
+        <v>42964</v>
+      </c>
+      <c r="M39" s="66"/>
+      <c r="N39" s="69">
+        <f t="shared" ref="N39:N41" si="44">MAX($Q$38:$Q$41)/SUBTOTAL(102,$Q$38:$Q$41)</f>
+        <v>12</v>
+      </c>
+      <c r="O39" s="48">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="49">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="50">
+        <f t="shared" si="33"/>
+        <v>48</v>
+      </c>
+      <c r="R39" s="50">
+        <f t="shared" si="34"/>
+        <v>-5068</v>
+      </c>
+      <c r="S39" s="50">
+        <f t="shared" si="42"/>
+        <v>-3040</v>
+      </c>
+      <c r="T39" s="50">
+        <f t="shared" si="35"/>
+        <v>3040</v>
+      </c>
+      <c r="U39" s="50">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="V39" s="51">
+        <f t="shared" si="43"/>
+        <v>0.59984214680347281</v>
+      </c>
+      <c r="W39" s="52" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X39" s="52" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y39" s="60">
+        <f t="shared" si="39"/>
+        <v>42962</v>
+      </c>
+      <c r="Z39" s="61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" s="56" customFormat="1">
+      <c r="A40" s="55">
+        <v>42962</v>
+      </c>
+      <c r="B40" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57">
+        <v>3533</v>
+      </c>
+      <c r="F40" s="57">
+        <v>0.6</v>
+      </c>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="57"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="58"/>
+      <c r="L40" s="55">
+        <v>42964</v>
+      </c>
+      <c r="M40" s="66"/>
+      <c r="N40" s="69">
+        <f t="shared" si="44"/>
+        <v>12</v>
+      </c>
+      <c r="O40" s="48">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="49">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q40" s="50">
+        <f t="shared" si="33"/>
+        <v>48</v>
+      </c>
+      <c r="R40" s="50">
+        <f t="shared" si="34"/>
+        <v>-3533</v>
+      </c>
+      <c r="S40" s="50">
+        <f t="shared" si="42"/>
+        <v>-2119</v>
+      </c>
+      <c r="T40" s="50">
+        <f t="shared" si="35"/>
+        <v>2119</v>
+      </c>
+      <c r="U40" s="50">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="V40" s="51">
+        <f t="shared" si="43"/>
+        <v>0.59977356354373057</v>
+      </c>
+      <c r="W40" s="52" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X40" s="52" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y40" s="60">
+        <f t="shared" si="39"/>
+        <v>42962</v>
+      </c>
+      <c r="Z40" s="61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" s="56" customFormat="1">
+      <c r="A41" s="55">
+        <v>42962</v>
+      </c>
+      <c r="B41" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57">
+        <v>4177</v>
+      </c>
+      <c r="F41" s="57">
+        <v>0.61</v>
+      </c>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="59"/>
+      <c r="K41" s="58"/>
+      <c r="L41" s="55">
+        <v>42964</v>
+      </c>
+      <c r="M41" s="66"/>
+      <c r="N41" s="69">
+        <f t="shared" si="44"/>
+        <v>12</v>
+      </c>
+      <c r="O41" s="48">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P41" s="49">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q41" s="50">
+        <f t="shared" si="33"/>
+        <v>48</v>
+      </c>
+      <c r="R41" s="50">
+        <f t="shared" si="34"/>
+        <v>-4177</v>
+      </c>
+      <c r="S41" s="50">
+        <f t="shared" si="42"/>
+        <v>-2547</v>
+      </c>
+      <c r="T41" s="50">
+        <f t="shared" si="35"/>
+        <v>2547</v>
+      </c>
+      <c r="U41" s="50">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="V41" s="51">
+        <f t="shared" si="43"/>
+        <v>0.60976777591572895</v>
+      </c>
+      <c r="W41" s="52" t="e">
+        <f t="shared" si="37"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X41" s="52" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y41" s="60">
+        <f t="shared" si="39"/>
+        <v>42962</v>
+      </c>
+      <c r="Z41" s="61" t="s">
         <v>376</v>
       </c>
     </row>

</xml_diff>